<commit_message>
Updating generator parsing, small changes to bnf.
</commit_message>
<xml_diff>
--- a/EXAMPLES/Examples.xlsx
+++ b/EXAMPLES/Examples.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="440" yWindow="-80" windowWidth="24100" windowHeight="15360" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="500" yWindow="-80" windowWidth="24100" windowHeight="15360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Untracked querying" sheetId="5" r:id="rId1"/>
@@ -21,62 +21,632 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="126">
+  <si>
+    <t>CREATE TABLE ChessBoard WITH BASE=board AS SELECT * FROM vector&lt;vector&lt;ChessPiece&gt; &gt;;-------</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE ChessRow AS SELECT * FROM vector&lt;ChessPiece&gt;;---------</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CREATE TABLE myVehicles WITH BASE=my_vehicles AS SELECT * FROM map&lt;string,Vehicle&gt;;----------- </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE theTime WITH BASE=theTime AS SELECT * FROM tm*;------------------------------------------------------------------------------- CREATE VIEW TimeView AS SELECT * FROM theTime, Time WHERE Time.base=theTime.time_ptr;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE ChessBoard WITH BASE=board AS SELECT * FROM vector&lt;vector&lt;ChessPiece&gt; &gt;;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE ChessRow AS SELECT * FROM vector&lt;ChessPiece&gt;;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE myVehicles WITH BASE=my_vehicles AS SELECT * FROM map&lt;string,Vehicle&gt;;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE ELEMENT TABLE Vehicle (plate TEXT FROM plate, brand TEXT FROM get_brand(), model INT FROM model);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE theTime WITH BASE=theTime AS SELECT * FROM tm*;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE theTime (year INT, month INT, day INT, hours INT, minutes INT, seconds INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * FROM theTime;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE AddressId AS SELECT * FROM vector&lt;Address*&gt;;----------------------------------------------------- CREATE VIEW Directory AS SELECT * FROM AddressId, Location WHERE Location.base=AddressId.address_ptr;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE EmployeeVehicleID AS SELECT * FROM set&lt;Vehicle*&gt;;------------------------------------------------ CREATE VIEW EmployeeVehicleView AS SELECT * FROM EmployeeVehicleID, EVehicle WHERE EVehicle.base=EmployeeVehicleID.e_vehicle_ptr;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * FROM myVehicles;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE myVehicles (tag_name TEXT, plate TEXT, brand TEXT, model INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * FROM the company, Personnel WHERE Personnel.base = theCompany.c_personnel AND theCompany.name = 'Siemens';</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE ELEMENT TABLE Employee (name TEXT FROM name, surname TEXT FROM surname, age INT FROM age, e_phones INT FROM get_phones(), e_vehicles FROM get_vehicles());</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE ELEMENT TABLE ChessPiece ( name string FROM get_name(), color INT FROM color);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE ELEMENT TABLE ChessBoard (chess_row INT FROM self);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE ELEMENT TABLE ChessRow (chess_piece INT FROM self);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE ELEMENT TABLE tm (year INT FROM tm_year, month INT FROM tm_month, day INT FROM tm_mday, hours INT FROM tm_hour, minutes INT FROM tm_min, seconds INT FROM tm_sec);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE ELEMENT TABLE ChessPiece ( name string FROM get_name(), color INT FROM color);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CREATE ELEMENT TABLE ChessBoard (chess_row INT FROM </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>TABLE ChessRow WITH BASE=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>self);</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE ELEMENT TABLE Vehicle (plate TEXT FROM plate, brand TEXT FROM get_brand(), model INT FROM model);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE ELEMENT TABLE Address (street TEXT FROM get_street(), number TEXT FROM number, postcode TEXT FROM get_postcode());</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mould for pointers to Vehicle element</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE Evehicle AS SELECT * FROM Vehicle;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Record - Table</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE EVehicle (base INT, plate TEXT, brand TEXT, model INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE CPhoneNumber AS SELECT * FROM vector&lt;long int&gt;;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE CPhoneNumber (base INT, phone_number INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Look for an element table with the same name as the VT irrespective of the type ("AS SELECT * FROM &lt;type&gt;"). If there is no element table (that is no element table name matches (in)type or VT name): search for CREATE ELEMENT TABLE &lt;VTN&gt;.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE ELEMENT TABLE Address (street TEXT FROM get_street(), number TEXT FROM number, postcode TEXT FROM get_postcode());</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CREATE ELEMENT TABLE Employee (name TEXT FROM name, surname TEXT FROM surname, age INT FROM age, e_phones INT FROM </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>TABLE E_Phone_number WITH BASE=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t xml:space="preserve">get_phones(), e_vehicles FROM </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>TABLE EmployeeVehicleID WITH BASE=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>get_vehicles());</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * FROM theCompany, AddressID, Location WHERE Location.base = AddressId.address_ptr AND AddressId.base = theCompany.c_directory AND theCompany.name = 'Proton Bank';</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT Fleet.plate, Fleet.brand, Fleet.model FROM theCompany,Fleet WHERE Fleet.base = theCompany.c_fleet AND theCompany.name = 'Proton Bank';</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * FROM theCompany, Personnel, EVehicle, EmployeeVehicleID WHERE EVehicle.base=EmployeeVehicleId.e_vehicle_ptr AND EmployeeVehicleID.base = Personnel.e_vehicles AND Personnel.base = theCompany.c_personnel AND theCompany.name = 'Alter' AND Personnel.surname='Giannikos';</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * FROM theTime, Time WHERE time.base = theTime.time_ptr;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE theCompany (c_fleet INT, name TEXT, vat TEXT...);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>B. Namespace for global variables.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C. Use extern global variables all the way or any_dstr?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CREATE ELEMENT TABLE Company (c_fleet INT FROM </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>TABLE Fleet WITH BASE=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t xml:space="preserve">get_fleet(), name TEXT FROM name, c_directory INT FROM </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>TABLE AddressID WITH BASE=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t xml:space="preserve">get_directory(), vat TEXT FROM vat, c_personnel INT FROM </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>TABLE Personnel WITH BASE=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t xml:space="preserve">get_personnel(), c_phones INT FROM </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>TABLE C_Phone_number WITH BASE=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>get_phones());</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>A. Object, pointer mismatch for nested stl structs? As defined by user in C++.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE Home (street TEXT, number TEXT, postcode TEXT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>class Company { vector&lt;Vehicle&gt; c_fleet; name string; vector&lt;Address*&gt; c_directory; vat string; vector&lt;Employee&gt; c_personnel; vector&lt;long int&gt;c_phones; }</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE ChessPiece AS SELECT * FROM ChessPiece;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE ChessPiece (base INT, name STRING, color INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SQL CREATE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SQL SELECT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TABLE TYPE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Collection</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Record - Table</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE Home WITH BASE=home AS SELECT * FROM Address;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Record</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE AddressID (base INT, address_ptr INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CREATE ELEMENT TABLE Company (c_fleet INT FROM </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t xml:space="preserve">get_fleet(), name TEXT FROM name, c_directory INT FROM </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t xml:space="preserve">get_directory(), vat TEXT FROM vat, c_personnel INT FROM </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t xml:space="preserve">get_personnel(), c_phones INT FROM </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>get_phones());</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>map&lt;string,Vehicle&gt; my_vehicles;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE theCompany WITH BASE=theCompany AS SELECT * FROM Company;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C++</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DSL</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE Fleet AS SELECT * FROM vector&lt;Vehicle&gt;;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>in class Company: vector&lt;Vehicle&gt; c_fleet;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>in class Company: vector&lt;Address*&gt; c_directory;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>class ChessPiece { string name; int color;}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE theCompany (c_fleet INT, name TEXT, c_directory INT, vat TEXT, c_personnel INT, c_phones INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT theCompany.name FROM theCompany, Fleet WHERE Fleet.base=theCompany.c_fleet AND Fleet.plate LIKE '%99';</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Record</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE Fleet ( base INT, plate TEXT, brand TEXT, model INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE ELEMENT TABLE Vehicle ( plate TEXT FROM plate, brand TEXT FROM get_brand(), model INT FROM model)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector&lt;vector&lt;ChessPiece&gt; &gt; board;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Collection</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>do we support this?work with both built-in base and supplied? The built-in definition has to come first but still. By mixing embedded with stand-alone you disuse the approach used in bestindex to carry out joins in a manner that agrees with our rationale. In conclusion a VT instance is like a constant. It keeps its definition and reflects the same C/C++ entity throughout its lifetime. If it is defined stand-alone, or embedded, it stays that way.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT phone_number FROM the company, Personnel, EPhoneNumber WHERE Personnel.base=theCompany.c_personnel AND EPhoneNumber.base=Personnel.e_phones UNION SELECT phone_number FROM the company, CPhoneNumber WHERE CPhoneNumber.base=theCompany.c_phones;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE EPhoneNumber AS SELECT * FROM vector&lt;long int&gt;;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>class Company { vector&lt;Vehicle&gt; c_fleet; name string; vat string;... }</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CREATE ELEMENT TABLE Company ( c_fleet INT </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>FROM TABLE Fleet WITH BASE=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>get_fleet(), name TEXT FROM name, vat TEXT FROM vat;...)</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE Location (base INT, street TEXT, number TEXT, postcode TEXT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>class Address { string street; string number; string postcode; }</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;ctime.h&gt;                   struct tm { int tm_sec; int tm_min; int tm_hour; int tm_mday; int tm_mon; int tm_year;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">#include &lt;ctime.h&gt;        time_t currnt_t=time();   tm *theTime =localtime(currnt_t);                      </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Record - Table</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE EmployeeVehicleID (base INT, e_vehicle_ptr INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>in class Company: vector&lt;Employee&gt; c_personnel;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE Personnel AS SELECT * FROM vector&lt;Employee&gt;;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>in class Employee: set&lt;Vehicle*&gt; e_vehicles;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE Personnel (base INT, name TEXT, surname TEXT, age INT, e_phones INT, e_vehicles INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mould for pointers to tm element</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Record - Table</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE Time AS SELECT * FROM tm;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE Time (base INT, year INT, month INT, day INT, hours INT, minutes INT, seconds INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE theTime (time_ptr INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE ChessBoard (chess_row INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE ChessRow (base INT, chess_piece INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * FROM ChessBoard, ChessRow, ChessPiece WHERE ChessRow.base=ChessBoard.chess_row AND ChessPiece.base=ChessRow.chess_piece</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>in class Employee: vector&lt;long int&gt; e_phones;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>See below</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>in class Company: vector&lt;long int&gt; c_phones;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Record</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE Fleet AS SELECT * FROM vector&lt;Vehicle&gt;;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>class Employee {name string; surname string; age int; vector&lt;long int&gt; e_phones; set&lt;Vehicle*&gt; e_vehicles; }</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>class Vehicle {string plate;  string brand; int model; }</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE Fleet (base INT, plate TEXT, brand TEXT, model INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Company theCompany;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
   <si>
     <t>in class Company:  vector&lt;Vehicle&gt; c_fleet;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>CREATE ELEMENT TABLE myVehicles (tag_name STRING FROM self, #Vehicle);</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>CREATE ELEMENT TABLE EmployeeVehicleID (e_vehicle_ptr INT FROM self);</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>CREATE ELEMENT TABLE myVehicles (tag_name STRING FROM self, #Vehicle);</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>CREATE ELEMENT TABLE CPhoneNumber (phone_number INT FROM self);</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>CREATE ELEMENT TABLE EPhoneNumber (phone_number INT FROM self);</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>CREATE ELEMENT TABLE theTime (time_ptr INT FROM self);</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>CREATE ELEMENT TABLE CPhoneNumber (phone_number INT FROM self);</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>CREATE VIRTUAL TABLE EPhoneNumber (base INT, phone_number INT);</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE ChessBoard WITH BASE=board AS SELECT * FROM vector&lt;vector&lt;ChessPiece&gt; &gt;;     USE ELEMENT ChessBoard;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE ChessRow AS SELECT * FROM vector&lt;ChessPiece&gt;;       USE ELEMENT ChessRow;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>in board: vector&lt;ChessPiece&gt; chess_row;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>in board:             ChessPiece chess_p;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>in board:             ChessPiece chess_p;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -104,610 +674,52 @@
       </rPr>
       <t>self);</t>
     </r>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>CREATE ELEMENT TABLE AddressId (address_ptr INT FROM self;)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>*!*-----type in stl class------- What happens with associative e.g. map&lt;int, Vehicle&gt;?You can override the CREATE ELEMENT TABLE identified by type (explicit command 'USE' &lt;virtual_table_name&gt; right at the bottom of the CREATE TABLE) with CREATE ELEMENT TABLE identified by &lt;virtual_table_name&gt;. To autofill Vehicle we could define "#Vehicle".</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>CREATE ELEMENT TABLE AddressId (address_ptr INT FROM self);</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>CREATE ELEMENT TABLE EmployeeVehicleID (e_vehicle_ptr INT FROM self);</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>CREATE TABLE Location AS SELECT * FROM Address;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Address home;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>SELECT * FROM Home;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>mould for pointers to Address element</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE Location (base INT, street TEXT, number TEXT, postcode TEXT);</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>class Address { string street; string number; string postcode; }</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;ctime.h&gt;                   struct tm { int tm_sec; int tm_min; int tm_hour; int tm_mday; int tm_mon; int tm_year;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">#include &lt;ctime.h&gt;        time_t currnt_t=time();   tm *theTime =localtime(currnt_t);                      </t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Record - Table</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE EmployeeVehicleID (base INT, e_vehicle_ptr INT);</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>in class Company: vector&lt;Employee&gt; c_personnel;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE Personnel AS SELECT * FROM vector&lt;Employee&gt;;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>in class Employee: set&lt;Vehicle*&gt; e_vehicles;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE Personnel (base INT, name TEXT, surname TEXT, age INT, e_phones INT, e_vehicles INT);</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>mould for pointers to tm element</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Record - Table</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE Time AS SELECT * FROM tm;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE Time (base INT, year INT, month INT, day INT, hours INT, minutes INT, seconds INT);</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE theTime (time_ptr INT);</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE ChessBoard (chess_row INT);</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE ChessRow (base INT, chess_piece INT);</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT * FROM ChessBoard, ChessRow, ChessPiece WHERE ChessRow.base=ChessBoard.chess_row AND ChessPiece.base=ChessRow.chess_piece</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>in class Employee: vector&lt;long int&gt; e_phones;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>See below</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>in class Company: vector&lt;long int&gt; c_phones;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Record</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE Fleet AS SELECT * FROM vector&lt;Vehicle&gt;;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>class Employee {name string; surname string; age int; vector&lt;long int&gt; e_phones; set&lt;Vehicle*&gt; e_vehicles; }</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>class Vehicle {string plate;  string brand; int model; }</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE Fleet (base INT, plate TEXT, brand TEXT, model INT);</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Company theCompany;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE theCompany WITH BASE=theCompany AS SELECT * FROM Company;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>C++</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>DSL</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE Fleet AS SELECT * FROM vector&lt;Vehicle&gt;;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>in class Company: vector&lt;Vehicle&gt; c_fleet;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>in class Company: vector&lt;Address*&gt; c_directory;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>class ChessPiece { string name; int color;}</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE theCompany (c_fleet INT, name TEXT, c_directory INT, vat TEXT, c_personnel INT, c_phones INT);</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT theCompany.name FROM theCompany, Fleet WHERE Fleet.base=theCompany.c_fleet AND Fleet.plate LIKE '%99';</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Record</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE Fleet ( base INT, plate TEXT, brand TEXT, model INT);</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE ELEMENT TABLE Vehicle ( plate TEXT FROM plate, brand TEXT FROM get_brand(), model INT FROM model)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>vector&lt;vector&lt;ChessPiece&gt; &gt; board;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Collection</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>do we support this?work with both built-in base and supplied? The built-in definition has to come first but still. By mixing embedded with stand-alone you disuse the approach used in bestindex to carry out joins in a manner that agrees with our rationale. In conclusion a VT instance is like a constant. It keeps its definition and reflects the same C/C++ entity throughout its lifetime. If it is defined stand-alone, or embedded, it stays that way.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT phone_number FROM the company, Personnel, EPhoneNumber WHERE Personnel.base=theCompany.c_personnel AND EPhoneNumber.base=Personnel.e_phones UNION SELECT phone_number FROM the company, CPhoneNumber WHERE CPhoneNumber.base=theCompany.c_phones;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE EPhoneNumber AS SELECT * FROM vector&lt;long int&gt;;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>class Company { vector&lt;Vehicle&gt; c_fleet; name string; vat string;... }</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">CREATE ELEMENT TABLE Company ( c_fleet INT </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>FROM TABLE Fleet WITH BASE=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>get_fleet(), name TEXT FROM name, vat TEXT FROM vat;...)</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE theCompany (c_fleet INT, name TEXT, vat TEXT...);</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>B. Namespace for global variables.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>C. Use extern global variables all the way or any_dstr?</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">CREATE ELEMENT TABLE Company (c_fleet INT FROM </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>TABLE Fleet WITH BASE=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t xml:space="preserve">get_fleet(), name TEXT FROM name, c_directory INT FROM </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>TABLE AddressID WITH BASE=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t xml:space="preserve">get_directory(), vat TEXT FROM vat, c_personnel INT FROM </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>TABLE Personnel WITH BASE=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t xml:space="preserve">get_personnel(), c_phones INT FROM </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>TABLE C_Phone_number WITH BASE=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>get_phones());</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>A. Object, pointer mismatch for nested stl structs? As defined by user in C++.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE Home (street TEXT, number TEXT, postcode TEXT);</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>class Company { vector&lt;Vehicle&gt; c_fleet; name string; vector&lt;Address*&gt; c_directory; vat string; vector&lt;Employee&gt; c_personnel; vector&lt;long int&gt;c_phones; }</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE ChessPiece AS SELECT * FROM ChessPiece;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE ChessPiece (base INT, name STRING, color INT);</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SQL CREATE</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SQL SELECT</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>TABLE TYPE</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Collection</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Record - Table</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE Home WITH BASE=home AS SELECT * FROM Address;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Record</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE AddressID (base INT, address_ptr INT);</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">CREATE ELEMENT TABLE Company (c_fleet INT FROM </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t xml:space="preserve">get_fleet(), name TEXT FROM name, c_directory INT FROM </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t xml:space="preserve">get_directory(), vat TEXT FROM vat, c_personnel INT FROM </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t xml:space="preserve">get_personnel(), c_phones INT FROM </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>get_phones());</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>map&lt;string,Vehicle&gt; my_vehicles;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE AddressId AS SELECT * FROM vector&lt;Address*&gt;;          USE ELEMENT AddressID;------------------------------------------------------------------ CREATE VIEW Directory AS SELECT * FROM AddressId, Location WHERE Location.base=AddressId.address_ptr;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE EmployeeVehicleID AS SELECT * FROM set&lt;Vehicle*&gt;;    USE ELEMENT EmployeeVehicleId;--------------------------------------------------------- CREATE VIEW EmployeeVehicleView AS SELECT * FROM EmployeeVehicleID, EVehicle WHERE EVehicle.base=EmployeeVehicleID.e_vehicle_ptr;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>mould for pointers to Vehicle element</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE Evehicle AS SELECT * FROM Vehicle;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Record - Table</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE EVehicle (base INT, plate TEXT, brand TEXT, model INT);</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE CPhoneNumber AS SELECT * FROM vector&lt;long int&gt;;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE CPhoneNumber (base INT, phone_number INT);</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Look for an element table with the same name as the VT irrespective of the type ("AS SELECT * FROM &lt;type&gt;"). If there is no element table (that is no element table name matches (in)type or VT name): search for CREATE ELEMENT TABLE &lt;VTN&gt;.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE ELEMENT TABLE Address (street TEXT FROM get_street(), number TEXT FROM number, postcode TEXT FROM get_postcode());</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">CREATE ELEMENT TABLE Employee (name TEXT FROM name, surname TEXT FROM surname, age INT FROM age, e_phones INT FROM </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>TABLE E_Phone_number WITH BASE=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t xml:space="preserve">get_phones(), e_vehicles FROM </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>TABLE EmployeeVehicleID WITH BASE=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>get_vehicles());</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT * FROM theCompany, AddressID, Location WHERE Location.base = AddressId.address_ptr AND AddressId.base = theCompany.c_directory AND theCompany.name = 'Proton Bank';</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT Fleet.plate, Fleet.brand, Fleet.model FROM theCompany,Fleet WHERE Fleet.base = theCompany.c_fleet AND theCompany.name = 'Proton Bank';</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT * FROM theCompany, Personnel, EVehicle, EmployeeVehicleID WHERE EVehicle.base=EmployeeVehicleId.e_vehicle_ptr AND EmployeeVehicleID.base = Personnel.e_vehicles AND Personnel.base = theCompany.c_personnel AND theCompany.name = 'Alter' AND Personnel.surname='Giannikos';</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT * FROM theTime, Time WHERE time.base = theTime.time_ptr;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE myVehicles WITH BASE=my_vehicles AS SELECT * FROM map&lt;string,Vehicle&gt;;----------- USE ELEMENT myVehicles;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT * FROM myVehicles;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE myVehicles (tag_name TEXT, plate TEXT, brand TEXT, model INT);</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT * FROM the company, Personnel WHERE Personnel.base = theCompany.c_personnel AND theCompany.name = 'Siemens';</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE theTime WITH BASE=theTime AS SELECT * FROM tm*;---------------------------------USE ELEMENT theTime;------------------------------------------------------------------------------- CREATE VIEW TimeView AS SELECT * FROM theTime, Time WHERE Time.base=theTime.time_ptr;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE ELEMENT TABLE Employee (name TEXT FROM name, surname TEXT FROM surname, age INT FROM age, e_phones INT FROM get_phones(), e_vehicles FROM get_vehicles());</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE ELEMENT TABLE ChessPiece ( name string FROM get_name(), color INT FROM color);</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE ELEMENT TABLE ChessBoard (chess_row INT FROM self);</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE ELEMENT TABLE ChessRow (chess_piece INT FROM self);</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE ELEMENT TABLE tm (year INT FROM tm_year, month INT FROM tm_month, day INT FROM tm_mday, hours INT FROM tm_hour, minutes INT FROM tm_min, seconds INT FROM tm_sec);</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE ELEMENT TABLE ChessPiece ( name string FROM get_name(), color INT FROM color);</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">CREATE ELEMENT TABLE ChessBoard (chess_row INT FROM </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>TABLE ChessRow WITH BASE=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>self);</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE ELEMENT TABLE Vehicle (plate TEXT FROM plate, brand TEXT FROM get_brand(), model INT FROM model);</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE ELEMENT TABLE Address (street TEXT FROM get_street(), number TEXT FROM number, postcode TEXT FROM get_postcode());</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE ChessBoard WITH BASE=board AS SELECT * FROM vector&lt;vector&lt;ChessPiece&gt; &gt;;-------USE ELEMENT ChessBoard;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE ChessRow AS SELECT * FROM vector&lt;ChessPiece&gt;;---------USE ELEMENT ChessRow;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE ELEMENT TABLE Vehicle (plate TEXT FROM plate, brand TEXT FROM get_brand(), model INT FROM model);</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <name val="Verdana"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Verdana"/>
     </font>
@@ -887,13 +899,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1266,8 +1278,8 @@
   </sheetPr>
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1281,19 +1293,19 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17" thickBot="1">
       <c r="A1" s="4" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>80</v>
+        <v>48</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" thickTop="1" thickBot="1">
@@ -1305,310 +1317,310 @@
     </row>
     <row r="3" spans="1:7" ht="121" customHeight="1" thickTop="1" thickBot="1">
       <c r="A3" s="10" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>88</v>
+        <v>56</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="12"/>
     </row>
     <row r="4" spans="1:7" ht="71" customHeight="1" thickTop="1" thickBot="1">
       <c r="A4" s="10" t="s">
-        <v>50</v>
+        <v>104</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>27</v>
+        <v>81</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="71" customHeight="1" thickTop="1" thickBot="1">
       <c r="A5" s="10" t="s">
-        <v>48</v>
+        <v>102</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>117</v>
+        <v>23</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="12"/>
     </row>
     <row r="6" spans="1:7" ht="123" customHeight="1" thickTop="1" thickBot="1">
       <c r="A6" s="10" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>49</v>
+        <v>103</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>102</v>
+        <v>35</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>16</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="86" customHeight="1" thickTop="1" thickBot="1">
       <c r="A7" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>24</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>118</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="12"/>
       <c r="G7" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="132" thickTop="1" thickBot="1">
       <c r="A8" s="10" t="s">
-        <v>22</v>
+        <v>125</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>27</v>
+        <v>81</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>19</v>
+        <v>122</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>23</v>
+        <v>77</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>43</v>
+        <v>97</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="49" customHeight="1" thickTop="1" thickBot="1">
       <c r="A9" s="10"/>
       <c r="B9" s="11" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>15</v>
+        <v>118</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="12"/>
     </row>
     <row r="10" spans="1:7" ht="136" customHeight="1" thickTop="1" thickBot="1">
       <c r="A10" s="10" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>90</v>
+        <v>11</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>101</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="58" customHeight="1" thickTop="1" thickBot="1">
       <c r="A11" s="10" t="s">
-        <v>20</v>
+        <v>123</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>27</v>
+        <v>81</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>76</v>
+        <v>44</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>21</v>
+        <v>124</v>
       </c>
       <c r="F11" s="16"/>
     </row>
     <row r="12" spans="1:7" ht="102" customHeight="1" thickTop="1" thickBot="1">
       <c r="A12" s="10" t="s">
-        <v>47</v>
+        <v>101</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>110</v>
+        <v>16</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="12"/>
     </row>
     <row r="13" spans="1:7" ht="85" customHeight="1" thickTop="1" thickBot="1">
       <c r="A13" s="10" t="s">
-        <v>29</v>
+        <v>83</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>108</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="58" customHeight="1" thickTop="1" thickBot="1">
       <c r="A14" s="10" t="s">
-        <v>92</v>
+        <v>25</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>94</v>
+        <v>27</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>93</v>
+        <v>26</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>95</v>
+        <v>28</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>43</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="60" customHeight="1" thickTop="1" thickBot="1">
       <c r="A15" s="10"/>
       <c r="B15" s="11" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>18</v>
+        <v>121</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="12"/>
     </row>
     <row r="16" spans="1:7" ht="165" customHeight="1" thickTop="1" thickBot="1">
       <c r="A16" s="10" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>91</v>
+        <v>12</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
       <c r="F16" s="16"/>
     </row>
     <row r="17" spans="1:6" ht="55" customHeight="1" thickTop="1" thickBot="1">
       <c r="A17" s="10"/>
       <c r="B17" s="11" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>1</v>
+        <v>106</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="12"/>
     </row>
     <row r="18" spans="1:6" ht="72" customHeight="1" thickTop="1" thickBot="1">
       <c r="A18" s="10" t="s">
-        <v>89</v>
+        <v>57</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>27</v>
+        <v>81</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>105</v>
+        <v>6</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>107</v>
+        <v>14</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>106</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="55" customHeight="1" thickTop="1" thickBot="1">
       <c r="A19" s="10"/>
       <c r="B19" s="11" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>7</v>
+        <v>112</v>
       </c>
       <c r="D19" s="11"/>
       <c r="E19" s="12"/>
     </row>
     <row r="20" spans="1:6" ht="95" customHeight="1" thickTop="1" thickBot="1">
       <c r="A20" s="10" t="s">
-        <v>44</v>
+        <v>98</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>96</v>
+        <v>29</v>
       </c>
       <c r="D20" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="E20" s="12" t="s">
-        <v>43</v>
-      </c>
       <c r="F20" s="16" t="s">
-        <v>98</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="66" customHeight="1" thickTop="1" thickBot="1">
       <c r="A21" s="10"/>
       <c r="B21" s="11" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
       <c r="D21" s="11"/>
       <c r="E21" s="12"/>
     </row>
     <row r="22" spans="1:6" ht="166" customHeight="1" thickTop="1" thickBot="1">
       <c r="A22" s="10" t="s">
-        <v>42</v>
+        <v>96</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>8</v>
+        <v>113</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="F22" s="16"/>
     </row>
@@ -1622,60 +1634,60 @@
     </row>
     <row r="24" spans="1:6" ht="107" customHeight="1" thickTop="1" thickBot="1">
       <c r="A24" s="10" t="s">
-        <v>25</v>
+        <v>79</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>114</v>
+        <v>20</v>
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="12"/>
     </row>
     <row r="25" spans="1:6" ht="70" customHeight="1" thickTop="1" thickBot="1">
       <c r="A25" s="10" t="s">
-        <v>33</v>
+        <v>87</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>34</v>
+        <v>88</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>35</v>
+        <v>89</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>36</v>
+        <v>90</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>43</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="96" customHeight="1" thickTop="1" thickBot="1">
       <c r="A26" s="10"/>
       <c r="B26" s="11" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>6</v>
+        <v>111</v>
       </c>
       <c r="D26" s="11"/>
       <c r="E26" s="12"/>
     </row>
     <row r="27" spans="1:6" ht="139" customHeight="1" thickTop="1" thickBot="1">
       <c r="A27" s="10" t="s">
-        <v>26</v>
+        <v>80</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>27</v>
+        <v>81</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>109</v>
+        <v>3</v>
       </c>
       <c r="D27" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27" s="12" t="s">
         <v>37</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="24" customHeight="1" thickTop="1" thickBot="1">
@@ -1687,13 +1699,13 @@
     </row>
     <row r="29" spans="1:6" ht="96" customHeight="1" thickTop="1" thickBot="1">
       <c r="A29" s="10" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>111</v>
+        <v>17</v>
       </c>
       <c r="D29" s="11"/>
       <c r="E29" s="12"/>
@@ -1701,10 +1713,10 @@
     <row r="30" spans="1:6" ht="96" customHeight="1" thickTop="1" thickBot="1">
       <c r="A30" s="10"/>
       <c r="B30" s="11" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="D30" s="11"/>
       <c r="E30" s="12"/>
@@ -1712,67 +1724,67 @@
     <row r="31" spans="1:6" ht="96" customHeight="1" thickTop="1" thickBot="1">
       <c r="A31" s="10"/>
       <c r="B31" s="11" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>112</v>
+        <v>18</v>
       </c>
       <c r="D31" s="11"/>
       <c r="E31" s="12"/>
     </row>
     <row r="32" spans="1:6" ht="68" customHeight="1" thickTop="1" thickBot="1">
       <c r="A32" s="10" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>38</v>
+        <v>92</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>43</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="60" customHeight="1" thickTop="1" thickBot="1">
       <c r="A33" s="10" t="s">
-        <v>11</v>
+        <v>114</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>39</v>
+        <v>93</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>43</v>
+        <v>97</v>
       </c>
       <c r="F33" s="16"/>
     </row>
     <row r="34" spans="1:6" ht="99" customHeight="1" thickTop="1" thickBot="1">
       <c r="A34" s="13" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>27</v>
+        <v>81</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="E34" s="15" t="s">
-        <v>40</v>
+        <v>94</v>
       </c>
       <c r="F34" t="s">
-        <v>41</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1784,7 +1796,7 @@
     </row>
     <row r="36" spans="1:6" ht="25" customHeight="1">
       <c r="A36" s="18" t="s">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="B36" s="18"/>
       <c r="C36" s="18"/>
@@ -1793,7 +1805,7 @@
     </row>
     <row r="37" spans="1:6" ht="21" customHeight="1">
       <c r="A37" s="18" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
       <c r="B37" s="18"/>
       <c r="C37" s="18"/>
@@ -1802,7 +1814,7 @@
     </row>
     <row r="38" spans="1:6" ht="27" customHeight="1">
       <c r="A38" s="18" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="B38" s="18"/>
       <c r="C38" s="18"/>
@@ -1887,12 +1899,13 @@
       <c r="E49" s="1"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="3">
     <mergeCell ref="A36:E36"/>
     <mergeCell ref="A37:E37"/>
     <mergeCell ref="A38:E38"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75196850393700787" right="0.75196850393700787" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" scale="39" fitToHeight="2" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -1910,7 +1923,7 @@
   </sheetPr>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1925,19 +1938,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17" thickBot="1">
       <c r="A1" s="4" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>80</v>
+        <v>48</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" thickTop="1" thickBot="1">
@@ -1949,65 +1962,66 @@
     </row>
     <row r="3" spans="1:5" ht="90" customHeight="1" thickTop="1" thickBot="1">
       <c r="A3" s="10" t="s">
-        <v>48</v>
+        <v>102</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="12"/>
     </row>
     <row r="4" spans="1:5" ht="79" customHeight="1" thickTop="1" thickBot="1">
       <c r="A4" s="10" t="s">
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>83</v>
+        <v>51</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>46</v>
+        <v>100</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="E4" s="12"/>
     </row>
     <row r="5" spans="1:5" ht="85" customHeight="1" thickTop="1" thickBot="1">
       <c r="A5" s="10" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="12"/>
     </row>
     <row r="6" spans="1:5" ht="106" customHeight="1" thickTop="1" thickBot="1">
       <c r="A6" s="10" t="s">
-        <v>50</v>
+        <v>104</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="14" thickTop="1"/>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75196850393700787" right="0.75196850393700787" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -2024,8 +2038,8 @@
   </sheetPr>
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -2039,19 +2053,19 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17" thickBot="1">
       <c r="A1" s="4" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>80</v>
+        <v>48</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" thickTop="1" thickBot="1">
@@ -2063,310 +2077,310 @@
     </row>
     <row r="3" spans="1:7" ht="177" customHeight="1" thickTop="1" thickBot="1">
       <c r="A3" s="10" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="12"/>
     </row>
     <row r="4" spans="1:7" ht="72" customHeight="1" thickTop="1" thickBot="1">
       <c r="A4" s="10" t="s">
-        <v>50</v>
+        <v>104</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>27</v>
+        <v>81</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A5" s="10" t="s">
-        <v>48</v>
+        <v>102</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>121</v>
+        <v>7</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="12"/>
     </row>
     <row r="6" spans="1:7" ht="121" customHeight="1" thickTop="1" thickBot="1">
       <c r="A6" s="10" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>49</v>
+        <v>103</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>102</v>
+        <v>35</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>16</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="76" customHeight="1" thickTop="1" thickBot="1">
       <c r="A7" s="10" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>99</v>
+        <v>32</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="12"/>
       <c r="G7" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="150" customHeight="1" thickTop="1" thickBot="1">
       <c r="A8" s="10" t="s">
-        <v>22</v>
+        <v>125</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>27</v>
+        <v>81</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>19</v>
+        <v>122</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>23</v>
+        <v>77</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>43</v>
+        <v>97</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="96" customHeight="1" thickTop="1" thickBot="1">
       <c r="A9" s="10"/>
       <c r="B9" s="11" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>17</v>
+        <v>120</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="12"/>
     </row>
     <row r="10" spans="1:7" ht="142" customHeight="1" thickTop="1" thickBot="1">
       <c r="A10" s="10" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>90</v>
+        <v>11</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>101</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="66" customHeight="1" thickTop="1" thickBot="1">
       <c r="A11" s="10" t="s">
-        <v>20</v>
+        <v>123</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>27</v>
+        <v>81</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>76</v>
+        <v>44</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>21</v>
+        <v>124</v>
       </c>
       <c r="F11" s="16"/>
     </row>
     <row r="12" spans="1:7" ht="128" customHeight="1" thickTop="1" thickBot="1">
       <c r="A12" s="10" t="s">
-        <v>47</v>
+        <v>101</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>100</v>
+        <v>33</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="12"/>
     </row>
     <row r="13" spans="1:7" ht="85" customHeight="1" thickTop="1" thickBot="1">
       <c r="A13" s="10" t="s">
-        <v>29</v>
+        <v>83</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>108</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="96" customHeight="1" thickTop="1" thickBot="1">
       <c r="A14" s="10" t="s">
-        <v>92</v>
+        <v>25</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>94</v>
+        <v>27</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>93</v>
+        <v>26</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>95</v>
+        <v>28</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>43</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="96" customHeight="1" thickTop="1" thickBot="1">
       <c r="A15" s="10"/>
       <c r="B15" s="11" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>2</v>
+        <v>107</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="12"/>
     </row>
     <row r="16" spans="1:7" ht="169" customHeight="1" thickTop="1" thickBot="1">
       <c r="A16" s="10" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>91</v>
+        <v>12</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
       <c r="F16" s="16"/>
     </row>
     <row r="17" spans="1:6" ht="55" customHeight="1" thickTop="1" thickBot="1">
       <c r="A17" s="10"/>
       <c r="B17" s="11" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>3</v>
+        <v>108</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="12"/>
     </row>
     <row r="18" spans="1:6" ht="72" customHeight="1" thickTop="1" thickBot="1">
       <c r="A18" s="10" t="s">
-        <v>89</v>
+        <v>57</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>27</v>
+        <v>81</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>105</v>
+        <v>2</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>107</v>
+        <v>14</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>106</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="55" customHeight="1" thickTop="1" thickBot="1">
       <c r="A19" s="10"/>
       <c r="B19" s="11" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>4</v>
+        <v>109</v>
       </c>
       <c r="D19" s="11"/>
       <c r="E19" s="12"/>
     </row>
     <row r="20" spans="1:6" ht="95" customHeight="1" thickTop="1" thickBot="1">
       <c r="A20" s="10" t="s">
-        <v>44</v>
+        <v>98</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>96</v>
+        <v>29</v>
       </c>
       <c r="D20" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="E20" s="12" t="s">
-        <v>43</v>
-      </c>
       <c r="F20" s="16" t="s">
-        <v>98</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="96" customHeight="1" thickTop="1" thickBot="1">
       <c r="A21" s="10"/>
       <c r="B21" s="11" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
       <c r="D21" s="11"/>
       <c r="E21" s="12"/>
     </row>
     <row r="22" spans="1:6" ht="177" customHeight="1" thickTop="1" thickBot="1">
       <c r="A22" s="10" t="s">
-        <v>42</v>
+        <v>96</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>8</v>
+        <v>113</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="F22" s="16"/>
     </row>
@@ -2380,278 +2394,254 @@
     </row>
     <row r="24" spans="1:6" ht="107" customHeight="1" thickTop="1" thickBot="1">
       <c r="A24" s="10" t="s">
-        <v>25</v>
+        <v>79</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>114</v>
+        <v>20</v>
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="12"/>
     </row>
-    <row r="25" spans="1:6" ht="79" customHeight="1" thickTop="1" thickBot="1">
+    <row r="25" spans="1:6" ht="139" customHeight="1" thickTop="1" thickBot="1">
       <c r="A25" s="10" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="96" customHeight="1" thickTop="1" thickBot="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="24" customHeight="1" thickTop="1" thickBot="1">
       <c r="A26" s="10"/>
-      <c r="B26" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>6</v>
-      </c>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
       <c r="D26" s="11"/>
       <c r="E26" s="12"/>
     </row>
-    <row r="27" spans="1:6" ht="139" customHeight="1" thickTop="1" thickBot="1">
+    <row r="27" spans="1:6" ht="67" customHeight="1" thickTop="1" thickBot="1">
       <c r="A27" s="10" t="s">
-        <v>26</v>
+        <v>64</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="24" customHeight="1" thickTop="1" thickBot="1">
+        <v>21</v>
+      </c>
+      <c r="D27" s="11"/>
+      <c r="E27" s="12"/>
+    </row>
+    <row r="28" spans="1:6" ht="70" customHeight="1" thickTop="1" thickBot="1">
       <c r="A28" s="10"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
+      <c r="B28" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>117</v>
+      </c>
       <c r="D28" s="11"/>
       <c r="E28" s="12"/>
     </row>
-    <row r="29" spans="1:6" ht="67" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A29" s="10" t="s">
-        <v>57</v>
-      </c>
+    <row r="29" spans="1:6" ht="66" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A29" s="10"/>
       <c r="B29" s="11" t="s">
-        <v>60</v>
+        <v>99</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>115</v>
+        <v>22</v>
       </c>
       <c r="D29" s="11"/>
       <c r="E29" s="12"/>
     </row>
-    <row r="30" spans="1:6" ht="70" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A30" s="10"/>
+    <row r="30" spans="1:6" ht="71" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A30" s="10" t="s">
+        <v>70</v>
+      </c>
       <c r="B30" s="11" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D30" s="11"/>
-      <c r="E30" s="12"/>
-    </row>
-    <row r="31" spans="1:6" ht="66" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A31" s="10"/>
+        <v>0</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="58" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A31" s="10" t="s">
+        <v>114</v>
+      </c>
       <c r="B31" s="11" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="C31" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="F31" s="16"/>
+    </row>
+    <row r="32" spans="1:6" ht="99" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A32" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="D31" s="11"/>
-      <c r="E31" s="12"/>
-    </row>
-    <row r="32" spans="1:6" ht="71" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A32" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="E32" s="12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="58" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A33" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="D33" s="11" t="s">
+      <c r="B32" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="F32" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="1:5" ht="25" customHeight="1">
+      <c r="A34" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+    </row>
+    <row r="35" spans="1:5" ht="21" customHeight="1">
+      <c r="A35" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="E33" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="F33" s="16"/>
-    </row>
-    <row r="34" spans="1:6" ht="99" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A34" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B34" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C34" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="D34" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="E34" s="15" t="s">
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+    </row>
+    <row r="36" spans="1:5" ht="27" customHeight="1">
+      <c r="A36" s="18" t="s">
         <v>40</v>
-      </c>
-      <c r="F34" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-    </row>
-    <row r="36" spans="1:6" ht="25" customHeight="1">
-      <c r="A36" s="18" t="s">
-        <v>74</v>
       </c>
       <c r="B36" s="18"/>
       <c r="C36" s="18"/>
       <c r="D36" s="18"/>
       <c r="E36" s="18"/>
     </row>
-    <row r="37" spans="1:6" ht="21" customHeight="1">
-      <c r="A37" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-    </row>
-    <row r="38" spans="1:6" ht="27" customHeight="1">
-      <c r="A38" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-    </row>
-    <row r="40" spans="1:6">
+    <row r="37" spans="1:5">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:5">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:5">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:5">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:5">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:5">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:5">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
     </row>
-    <row r="47" spans="1:6">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="A48" s="3"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+    </row>
+    <row r="48" spans="1:5" ht="16"/>
+    <row r="49" ht="16"/>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="3">
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="A35:E35"/>
     <mergeCell ref="A36:E36"/>
-    <mergeCell ref="A37:E37"/>
-    <mergeCell ref="A38:E38"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75196850393700787" right="0.75196850393700787" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Committing files necessary to build and/or comprehend each example. Updated Examples.xslx. Untrack stl_search.cpp from SOURCE since it is derived.
</commit_message>
<xml_diff>
--- a/EXAMPLES/Examples.xlsx
+++ b/EXAMPLES/Examples.xlsx
@@ -21,69 +21,546 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="126">
-  <si>
-    <t>CREATE TABLE ChessBoard WITH BASE=board AS SELECT * FROM vector&lt;vector&lt;ChessPiece&gt; &gt;;-------</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE ChessRow AS SELECT * FROM vector&lt;ChessPiece&gt;;---------</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">CREATE TABLE myVehicles WITH BASE=my_vehicles AS SELECT * FROM map&lt;string,Vehicle&gt;;----------- </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE theTime WITH BASE=theTime AS SELECT * FROM tm*;------------------------------------------------------------------------------- CREATE VIEW TimeView AS SELECT * FROM theTime, Time WHERE Time.base=theTime.time_ptr;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE ChessBoard WITH BASE=board AS SELECT * FROM vector&lt;vector&lt;ChessPiece&gt; &gt;;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE ChessRow AS SELECT * FROM vector&lt;ChessPiece&gt;;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE myVehicles WITH BASE=my_vehicles AS SELECT * FROM map&lt;string,Vehicle&gt;;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE ELEMENT TABLE Vehicle (plate TEXT FROM plate, brand TEXT FROM get_brand(), model INT FROM model);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE theTime WITH BASE=theTime AS SELECT * FROM tm*;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE theTime (year INT, month INT, day INT, hours INT, minutes INT, seconds INT);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT * FROM theTime;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE AddressId AS SELECT * FROM vector&lt;Address*&gt;;----------------------------------------------------- CREATE VIEW Directory AS SELECT * FROM AddressId, Location WHERE Location.base=AddressId.address_ptr;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE EmployeeVehicleID AS SELECT * FROM set&lt;Vehicle*&gt;;------------------------------------------------ CREATE VIEW EmployeeVehicleView AS SELECT * FROM EmployeeVehicleID, EVehicle WHERE EVehicle.base=EmployeeVehicleID.e_vehicle_ptr;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT * FROM myVehicles;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE myVehicles (tag_name TEXT, plate TEXT, brand TEXT, model INT);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT * FROM the company, Personnel WHERE Personnel.base = theCompany.c_personnel AND theCompany.name = 'Siemens';</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="125">
+  <si>
+    <t>CREATE ELEMENT TABLE EmployeeVehicleID (e_vehicle_ptr INT FROM self);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE Location AS SELECT * FROM Address;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Address home;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * FROM Home;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mould for pointers to Address element</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE ChessRow (base INT, name STRING, color INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE ELEMENT TABLE ChessRow ( name string FROM get_name(), color INT FROM color);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>in class Employee: vector&lt;long int&gt; e_phones;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>See below</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>in class Company: vector&lt;long int&gt; c_phones;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Record</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE Fleet AS SELECT * FROM vector&lt;Vehicle&gt;;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>class Employee {name string; surname string; age int; vector&lt;long int&gt; e_phones; set&lt;Vehicle*&gt; e_vehicles; }</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>class Vehicle {string plate;  string brand; int model; }</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE Fleet (base INT, plate TEXT, brand TEXT, model INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Company theCompany;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>in class Company:  vector&lt;Vehicle&gt; c_fleet;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE ELEMENT TABLE myVehicles (tag_name STRING FROM self, #Vehicle);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE ELEMENT TABLE EmployeeVehicleID (e_vehicle_ptr INT FROM self);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE ELEMENT TABLE myVehicles (tag_name STRING FROM self, #Vehicle);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE ELEMENT TABLE CPhoneNumber (phone_number INT FROM self);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE ELEMENT TABLE EPhoneNumber (phone_number INT FROM self);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE ELEMENT TABLE theTime (time_ptr INT FROM self);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE ELEMENT TABLE CPhoneNumber (phone_number INT FROM self);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE EPhoneNumber (base INT, phone_number INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>in board: vector&lt;ChessPiece&gt; chess_row;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>in board:             ChessPiece chess_p;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CREATE ELEMENT TABLE ChessRow (chess_piece INT </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>FROM</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t xml:space="preserve"> TABLE ChessPiece WITH BASE=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>self);</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE ELEMENT TABLE AddressId (address_ptr INT FROM self;)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>*!*-----type in stl class------- What happens with associative e.g. map&lt;int, Vehicle&gt;?You can override the CREATE ELEMENT TABLE identified by type (explicit command 'USE' &lt;virtual_table_name&gt; right at the bottom of the CREATE TABLE) with CREATE ELEMENT TABLE identified by &lt;virtual_table_name&gt;. To autofill Vehicle we could define "#Vehicle".</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE ELEMENT TABLE AddressId (address_ptr INT FROM self);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT phone_number FROM the company, Personnel, EPhoneNumber WHERE Personnel.base=theCompany.c_personnel AND EPhoneNumber.base=Personnel.e_phones UNION SELECT phone_number FROM the company, CPhoneNumber WHERE CPhoneNumber.base=theCompany.c_phones;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE EPhoneNumber AS SELECT * FROM vector&lt;long int&gt;;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>class Company { vector&lt;Vehicle&gt; c_fleet; name string; vat string;... }</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CREATE ELEMENT TABLE Company ( c_fleet INT </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>FROM TABLE Fleet WITH BASE=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>get_fleet(), name TEXT FROM name, vat TEXT FROM vat;...)</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE Location (base INT, street TEXT, number TEXT, postcode TEXT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>class Address { string street; string number; string postcode; }</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;ctime.h&gt;                   struct tm { int tm_sec; int tm_min; int tm_hour; int tm_mday; int tm_mon; int tm_year;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">#include &lt;ctime.h&gt;        time_t currnt_t=time();   tm *theTime =localtime(currnt_t);                      </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Record - Table</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE EmployeeVehicleID (base INT, e_vehicle_ptr INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>in class Company: vector&lt;Employee&gt; c_personnel;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE Personnel AS SELECT * FROM vector&lt;Employee&gt;;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>in class Employee: set&lt;Vehicle*&gt; e_vehicles;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE Personnel (base INT, name TEXT, surname TEXT, age INT, e_phones INT, e_vehicles INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mould for pointers to tm element</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Record - Table</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE Time AS SELECT * FROM tm;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE Time (base INT, year INT, month INT, day INT, hours INT, minutes INT, seconds INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE theTime (time_ptr INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE ChessBoard (chess_row INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE ChessRow (base INT, chess_piece INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * FROM ChessBoard, ChessRow, ChessPiece WHERE ChessRow.base=ChessBoard.chess_row AND ChessPiece.base=ChessRow.chess_piece</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SQL CREATE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SQL SELECT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TABLE TYPE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Collection</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Record - Table</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE Home WITH BASE=home AS SELECT * FROM Address;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Record</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE AddressID (base INT, address_ptr INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CREATE ELEMENT TABLE Company (c_fleet INT FROM </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t xml:space="preserve">get_fleet(), name TEXT FROM name, c_directory INT FROM </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t xml:space="preserve">get_directory(), vat TEXT FROM vat, c_personnel INT FROM </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t xml:space="preserve">get_personnel(), c_phones INT FROM </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>get_phones());</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>map&lt;string,Vehicle&gt; my_vehicles;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE theCompany WITH BASE=theCompany AS SELECT * FROM Company;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C++</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DSL</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE Fleet AS SELECT * FROM vector&lt;Vehicle&gt;;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>in class Company: vector&lt;Vehicle&gt; c_fleet;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>in class Company: vector&lt;Address*&gt; c_directory;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>class ChessPiece { string name; int color;}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE theCompany (c_fleet INT, name TEXT, c_directory INT, vat TEXT, c_personnel INT, c_phones INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT theCompany.name FROM theCompany, Fleet WHERE Fleet.base=theCompany.c_fleet AND Fleet.plate LIKE '%99';</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Record</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE Fleet ( base INT, plate TEXT, brand TEXT, model INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE ELEMENT TABLE Vehicle ( plate TEXT FROM plate, brand TEXT FROM get_brand(), model INT FROM model)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector&lt;vector&lt;ChessPiece&gt; &gt; board;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Collection</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>do we support this?work with both built-in base and supplied? The built-in definition has to come first but still. By mixing embedded with stand-alone you disuse the approach used in bestindex to carry out joins in a manner that agrees with our rationale. In conclusion a VT instance is like a constant. It keeps its definition and reflects the same C/C++ entity throughout its lifetime. If it is defined stand-alone, or embedded, it stays that way.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CREATE ELEMENT TABLE Employee (name TEXT FROM name, surname TEXT FROM surname, age INT FROM age, e_phones INT FROM </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>TABLE E_Phone_number WITH BASE=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t xml:space="preserve">get_phones(), e_vehicles FROM </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>TABLE EmployeeVehicleID WITH BASE=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>get_vehicles());</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * FROM theCompany, AddressID, Location WHERE Location.base = AddressId.address_ptr AND AddressId.base = theCompany.c_directory AND theCompany.name = 'Proton Bank';</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT Fleet.plate, Fleet.brand, Fleet.model FROM theCompany,Fleet WHERE Fleet.base = theCompany.c_fleet AND theCompany.name = 'Proton Bank';</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * FROM theCompany, Personnel, EVehicle, EmployeeVehicleID WHERE EVehicle.base=EmployeeVehicleId.e_vehicle_ptr AND EmployeeVehicleID.base = Personnel.e_vehicles AND Personnel.base = theCompany.c_personnel AND theCompany.name = 'Alter' AND Personnel.surname='Giannikos';</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * FROM theTime, Time WHERE time.base = theTime.time_ptr;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE theCompany (c_fleet INT, name TEXT, vat TEXT...);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>B. Namespace for global variables.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C. Use extern global variables all the way or any_dstr?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CREATE ELEMENT TABLE Company (c_fleet INT FROM </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>TABLE Fleet WITH BASE=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t xml:space="preserve">get_fleet(), name TEXT FROM name, c_directory INT FROM </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>TABLE AddressID WITH BASE=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t xml:space="preserve">get_directory(), vat TEXT FROM vat, c_personnel INT FROM </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>TABLE Personnel WITH BASE=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t xml:space="preserve">get_personnel(), c_phones INT FROM </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>TABLE C_Phone_number WITH BASE=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>get_phones());</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>A. Object, pointer mismatch for nested stl structs? As defined by user in C++.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE Home (street TEXT, number TEXT, postcode TEXT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>class Company { vector&lt;Vehicle&gt; c_fleet; name string; vector&lt;Address*&gt; c_directory; vat string; vector&lt;Employee&gt; c_personnel; vector&lt;long int&gt;c_phones; }</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE ChessPiece AS SELECT * FROM ChessPiece;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE ChessPiece (base INT, name STRING, color INT);</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -91,15 +568,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>CREATE ELEMENT TABLE ChessPiece ( name string FROM get_name(), color INT FROM color);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>CREATE ELEMENT TABLE ChessBoard (chess_row INT FROM self);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE ELEMENT TABLE ChessRow (chess_piece INT FROM self);</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -172,540 +641,67 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">CREATE ELEMENT TABLE Employee (name TEXT FROM name, surname TEXT FROM surname, age INT FROM age, e_phones INT FROM </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>TABLE E_Phone_number WITH BASE=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t xml:space="preserve">get_phones(), e_vehicles FROM </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>TABLE EmployeeVehicleID WITH BASE=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>get_vehicles());</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT * FROM theCompany, AddressID, Location WHERE Location.base = AddressId.address_ptr AND AddressId.base = theCompany.c_directory AND theCompany.name = 'Proton Bank';</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT Fleet.plate, Fleet.brand, Fleet.model FROM theCompany,Fleet WHERE Fleet.base = theCompany.c_fleet AND theCompany.name = 'Proton Bank';</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT * FROM theCompany, Personnel, EVehicle, EmployeeVehicleID WHERE EVehicle.base=EmployeeVehicleId.e_vehicle_ptr AND EmployeeVehicleID.base = Personnel.e_vehicles AND Personnel.base = theCompany.c_personnel AND theCompany.name = 'Alter' AND Personnel.surname='Giannikos';</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT * FROM theTime, Time WHERE time.base = theTime.time_ptr;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE theCompany (c_fleet INT, name TEXT, vat TEXT...);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>B. Namespace for global variables.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>C. Use extern global variables all the way or any_dstr?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">CREATE ELEMENT TABLE Company (c_fleet INT FROM </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>TABLE Fleet WITH BASE=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t xml:space="preserve">get_fleet(), name TEXT FROM name, c_directory INT FROM </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>TABLE AddressID WITH BASE=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t xml:space="preserve">get_directory(), vat TEXT FROM vat, c_personnel INT FROM </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>TABLE Personnel WITH BASE=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t xml:space="preserve">get_personnel(), c_phones INT FROM </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>TABLE C_Phone_number WITH BASE=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>get_phones());</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>A. Object, pointer mismatch for nested stl structs? As defined by user in C++.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE Home (street TEXT, number TEXT, postcode TEXT);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>class Company { vector&lt;Vehicle&gt; c_fleet; name string; vector&lt;Address*&gt; c_directory; vat string; vector&lt;Employee&gt; c_personnel; vector&lt;long int&gt;c_phones; }</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE ChessPiece AS SELECT * FROM ChessPiece;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE ChessPiece (base INT, name STRING, color INT);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SQL CREATE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SQL SELECT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>TABLE TYPE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Collection</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Record - Table</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE Home WITH BASE=home AS SELECT * FROM Address;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Record</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE AddressID (base INT, address_ptr INT);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">CREATE ELEMENT TABLE Company (c_fleet INT FROM </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t xml:space="preserve">get_fleet(), name TEXT FROM name, c_directory INT FROM </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t xml:space="preserve">get_directory(), vat TEXT FROM vat, c_personnel INT FROM </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t xml:space="preserve">get_personnel(), c_phones INT FROM </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>get_phones());</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>map&lt;string,Vehicle&gt; my_vehicles;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE theCompany WITH BASE=theCompany AS SELECT * FROM Company;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>C++</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>DSL</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE Fleet AS SELECT * FROM vector&lt;Vehicle&gt;;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>in class Company: vector&lt;Vehicle&gt; c_fleet;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>in class Company: vector&lt;Address*&gt; c_directory;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>class ChessPiece { string name; int color;}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE theCompany (c_fleet INT, name TEXT, c_directory INT, vat TEXT, c_personnel INT, c_phones INT);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT theCompany.name FROM theCompany, Fleet WHERE Fleet.base=theCompany.c_fleet AND Fleet.plate LIKE '%99';</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Record</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE Fleet ( base INT, plate TEXT, brand TEXT, model INT);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE ELEMENT TABLE Vehicle ( plate TEXT FROM plate, brand TEXT FROM get_brand(), model INT FROM model)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>vector&lt;vector&lt;ChessPiece&gt; &gt; board;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Collection</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>do we support this?work with both built-in base and supplied? The built-in definition has to come first but still. By mixing embedded with stand-alone you disuse the approach used in bestindex to carry out joins in a manner that agrees with our rationale. In conclusion a VT instance is like a constant. It keeps its definition and reflects the same C/C++ entity throughout its lifetime. If it is defined stand-alone, or embedded, it stays that way.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT phone_number FROM the company, Personnel, EPhoneNumber WHERE Personnel.base=theCompany.c_personnel AND EPhoneNumber.base=Personnel.e_phones UNION SELECT phone_number FROM the company, CPhoneNumber WHERE CPhoneNumber.base=theCompany.c_phones;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE EPhoneNumber AS SELECT * FROM vector&lt;long int&gt;;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>class Company { vector&lt;Vehicle&gt; c_fleet; name string; vat string;... }</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">CREATE ELEMENT TABLE Company ( c_fleet INT </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>FROM TABLE Fleet WITH BASE=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>get_fleet(), name TEXT FROM name, vat TEXT FROM vat;...)</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE Location (base INT, street TEXT, number TEXT, postcode TEXT);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>class Address { string street; string number; string postcode; }</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;ctime.h&gt;                   struct tm { int tm_sec; int tm_min; int tm_hour; int tm_mday; int tm_mon; int tm_year;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">#include &lt;ctime.h&gt;        time_t currnt_t=time();   tm *theTime =localtime(currnt_t);                      </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Record - Table</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE EmployeeVehicleID (base INT, e_vehicle_ptr INT);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>in class Company: vector&lt;Employee&gt; c_personnel;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE Personnel AS SELECT * FROM vector&lt;Employee&gt;;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>in class Employee: set&lt;Vehicle*&gt; e_vehicles;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE Personnel (base INT, name TEXT, surname TEXT, age INT, e_phones INT, e_vehicles INT);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>mould for pointers to tm element</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Record - Table</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE Time AS SELECT * FROM tm;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE Time (base INT, year INT, month INT, day INT, hours INT, minutes INT, seconds INT);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE theTime (time_ptr INT);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE ChessBoard (chess_row INT);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE ChessRow (base INT, chess_piece INT);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT * FROM ChessBoard, ChessRow, ChessPiece WHERE ChessRow.base=ChessBoard.chess_row AND ChessPiece.base=ChessRow.chess_piece</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>in class Employee: vector&lt;long int&gt; e_phones;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>See below</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>in class Company: vector&lt;long int&gt; c_phones;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Record</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE Fleet AS SELECT * FROM vector&lt;Vehicle&gt;;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>class Employee {name string; surname string; age int; vector&lt;long int&gt; e_phones; set&lt;Vehicle*&gt; e_vehicles; }</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>class Vehicle {string plate;  string brand; int model; }</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE Fleet (base INT, plate TEXT, brand TEXT, model INT);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Company theCompany;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>in class Company:  vector&lt;Vehicle&gt; c_fleet;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE ELEMENT TABLE myVehicles (tag_name STRING FROM self, #Vehicle);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE ELEMENT TABLE EmployeeVehicleID (e_vehicle_ptr INT FROM self);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE ELEMENT TABLE myVehicles (tag_name STRING FROM self, #Vehicle);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE ELEMENT TABLE CPhoneNumber (phone_number INT FROM self);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE ELEMENT TABLE EPhoneNumber (phone_number INT FROM self);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE ELEMENT TABLE theTime (time_ptr INT FROM self);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE ELEMENT TABLE CPhoneNumber (phone_number INT FROM self);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE EPhoneNumber (base INT, phone_number INT);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>in board: vector&lt;ChessPiece&gt; chess_row;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>in board:             ChessPiece chess_p;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>in board:             ChessPiece chess_p;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">CREATE ELEMENT TABLE ChessRow (chess_piece INT </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>FROM</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t xml:space="preserve"> TABLE ChessPiece WITH BASE=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>self);</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE ELEMENT TABLE AddressId (address_ptr INT FROM self;)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>*!*-----type in stl class------- What happens with associative e.g. map&lt;int, Vehicle&gt;?You can override the CREATE ELEMENT TABLE identified by type (explicit command 'USE' &lt;virtual_table_name&gt; right at the bottom of the CREATE TABLE) with CREATE ELEMENT TABLE identified by &lt;virtual_table_name&gt;. To autofill Vehicle we could define "#Vehicle".</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE ELEMENT TABLE AddressId (address_ptr INT FROM self);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE ELEMENT TABLE EmployeeVehicleID (e_vehicle_ptr INT FROM self);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE Location AS SELECT * FROM Address;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Address home;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT * FROM Home;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>mould for pointers to Address element</t>
+    <t>CREATE TABLE ChessBoard WITH BASE=board AS SELECT * FROM vector&lt;vector&lt;ChessPiece&gt; &gt;;-------</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE ChessRow AS SELECT * FROM vector&lt;ChessPiece&gt;;---------</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CREATE TABLE myVehicles WITH BASE=my_vehicles AS SELECT * FROM map&lt;string,Vehicle&gt;;----------- </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE theTime WITH BASE=theTime AS SELECT * FROM tm*;------------------------------------------------------------------------------- CREATE VIEW TimeView AS SELECT * FROM theTime, Time WHERE Time.base=theTime.time_ptr;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE ChessBoard WITH BASE=board AS SELECT * FROM vector&lt;vector&lt;ChessPiece&gt; &gt;;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE ChessRow AS SELECT * FROM vector&lt;ChessPiece&gt;;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE myVehicles WITH BASE=my_vehicles AS SELECT * FROM map&lt;string,Vehicle&gt;;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE ELEMENT TABLE Vehicle (plate TEXT FROM plate, brand TEXT FROM get_brand(), model INT FROM model);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE theTime WITH BASE=theTime AS SELECT * FROM tm*;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE theTime (year INT, month INT, day INT, hours INT, minutes INT, seconds INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * FROM theTime;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE AddressId AS SELECT * FROM vector&lt;Address*&gt;;----------------------------------------------------- CREATE VIEW Directory AS SELECT * FROM AddressId, Location WHERE Location.base=AddressId.address_ptr;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE EmployeeVehicleID AS SELECT * FROM set&lt;Vehicle*&gt;;------------------------------------------------ CREATE VIEW EmployeeVehicleView AS SELECT * FROM EmployeeVehicleID, EVehicle WHERE EVehicle.base=EmployeeVehicleID.e_vehicle_ptr;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * FROM myVehicles;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE myVehicles (tag_name TEXT, plate TEXT, brand TEXT, model INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * FROM the company, Personnel WHERE Personnel.base = theCompany.c_personnel AND theCompany.name = 'Siemens';</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1279,7 +1275,7 @@
   <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="A30" sqref="A30:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1293,19 +1289,19 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17" thickBot="1">
       <c r="A1" s="4" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" thickTop="1" thickBot="1">
@@ -1317,310 +1313,310 @@
     </row>
     <row r="3" spans="1:7" ht="121" customHeight="1" thickTop="1" thickBot="1">
       <c r="A3" s="10" t="s">
-        <v>45</v>
+        <v>91</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="12"/>
     </row>
     <row r="4" spans="1:7" ht="71" customHeight="1" thickTop="1" thickBot="1">
       <c r="A4" s="10" t="s">
-        <v>104</v>
+        <v>15</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="71" customHeight="1" thickTop="1" thickBot="1">
       <c r="A5" s="10" t="s">
-        <v>102</v>
+        <v>13</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>23</v>
+        <v>99</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="12"/>
     </row>
     <row r="6" spans="1:7" ht="123" customHeight="1" thickTop="1" thickBot="1">
       <c r="A6" s="10" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>103</v>
+        <v>14</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>35</v>
+        <v>81</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>119</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="86" customHeight="1" thickTop="1" thickBot="1">
       <c r="A7" s="10" t="s">
-        <v>78</v>
+        <v>36</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>24</v>
+        <v>100</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="12"/>
       <c r="G7" t="s">
-        <v>43</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="132" thickTop="1" thickBot="1">
       <c r="A8" s="10" t="s">
-        <v>125</v>
+        <v>4</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>122</v>
+        <v>1</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>77</v>
+        <v>35</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="49" customHeight="1" thickTop="1" thickBot="1">
       <c r="A9" s="10"/>
       <c r="B9" s="11" t="s">
-        <v>99</v>
+        <v>10</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>118</v>
+        <v>28</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="12"/>
     </row>
     <row r="10" spans="1:7" ht="136" customHeight="1" thickTop="1" thickBot="1">
       <c r="A10" s="10" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>34</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="58" customHeight="1" thickTop="1" thickBot="1">
       <c r="A11" s="10" t="s">
-        <v>123</v>
+        <v>2</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>44</v>
+        <v>90</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>124</v>
+        <v>3</v>
       </c>
       <c r="F11" s="16"/>
     </row>
     <row r="12" spans="1:7" ht="102" customHeight="1" thickTop="1" thickBot="1">
       <c r="A12" s="10" t="s">
-        <v>101</v>
+        <v>12</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>16</v>
+        <v>94</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="12"/>
     </row>
     <row r="13" spans="1:7" ht="85" customHeight="1" thickTop="1" thickBot="1">
       <c r="A13" s="10" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>84</v>
+        <v>42</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>86</v>
+        <v>44</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>15</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="58" customHeight="1" thickTop="1" thickBot="1">
       <c r="A14" s="10" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>27</v>
+        <v>103</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>28</v>
+        <v>104</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="60" customHeight="1" thickTop="1" thickBot="1">
       <c r="A15" s="10"/>
       <c r="B15" s="11" t="s">
-        <v>99</v>
+        <v>10</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>121</v>
+        <v>0</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="12"/>
     </row>
     <row r="16" spans="1:7" ht="165" customHeight="1" thickTop="1" thickBot="1">
       <c r="A16" s="10" t="s">
-        <v>85</v>
+        <v>43</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>12</v>
+        <v>121</v>
       </c>
       <c r="D16" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="12" t="s">
         <v>82</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>36</v>
       </c>
       <c r="F16" s="16"/>
     </row>
     <row r="17" spans="1:6" ht="55" customHeight="1" thickTop="1" thickBot="1">
       <c r="A17" s="10"/>
       <c r="B17" s="11" t="s">
-        <v>99</v>
+        <v>10</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>106</v>
+        <v>17</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="12"/>
     </row>
     <row r="18" spans="1:6" ht="72" customHeight="1" thickTop="1" thickBot="1">
       <c r="A18" s="10" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>14</v>
+        <v>123</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>13</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="55" customHeight="1" thickTop="1" thickBot="1">
       <c r="A19" s="10"/>
       <c r="B19" s="11" t="s">
-        <v>99</v>
+        <v>10</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>112</v>
+        <v>23</v>
       </c>
       <c r="D19" s="11"/>
       <c r="E19" s="12"/>
     </row>
     <row r="20" spans="1:6" ht="95" customHeight="1" thickTop="1" thickBot="1">
       <c r="A20" s="10" t="s">
-        <v>98</v>
+        <v>9</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>29</v>
+        <v>105</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>30</v>
+        <v>106</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="66" customHeight="1" thickTop="1" thickBot="1">
       <c r="A21" s="10"/>
       <c r="B21" s="11" t="s">
-        <v>99</v>
+        <v>10</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>110</v>
+        <v>21</v>
       </c>
       <c r="D21" s="11"/>
       <c r="E21" s="12"/>
     </row>
     <row r="22" spans="1:6" ht="166" customHeight="1" thickTop="1" thickBot="1">
       <c r="A22" s="10" t="s">
-        <v>96</v>
+        <v>7</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>74</v>
+        <v>32</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>73</v>
+        <v>31</v>
       </c>
       <c r="F22" s="16"/>
     </row>
@@ -1634,60 +1630,60 @@
     </row>
     <row r="24" spans="1:6" ht="107" customHeight="1" thickTop="1" thickBot="1">
       <c r="A24" s="10" t="s">
-        <v>79</v>
+        <v>37</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="12"/>
     </row>
     <row r="25" spans="1:6" ht="70" customHeight="1" thickTop="1" thickBot="1">
       <c r="A25" s="10" t="s">
-        <v>87</v>
+        <v>45</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>88</v>
+        <v>46</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>89</v>
+        <v>47</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>90</v>
+        <v>48</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="96" customHeight="1" thickTop="1" thickBot="1">
       <c r="A26" s="10"/>
       <c r="B26" s="11" t="s">
-        <v>99</v>
+        <v>10</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>111</v>
+        <v>22</v>
       </c>
       <c r="D26" s="11"/>
       <c r="E26" s="12"/>
     </row>
     <row r="27" spans="1:6" ht="139" customHeight="1" thickTop="1" thickBot="1">
       <c r="A27" s="10" t="s">
-        <v>80</v>
+        <v>38</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>3</v>
+        <v>112</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>91</v>
+        <v>49</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="24" customHeight="1" thickTop="1" thickBot="1">
@@ -1699,13 +1695,13 @@
     </row>
     <row r="29" spans="1:6" ht="96" customHeight="1" thickTop="1" thickBot="1">
       <c r="A29" s="10" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D29" s="11"/>
       <c r="E29" s="12"/>
@@ -1713,197 +1709,167 @@
     <row r="30" spans="1:6" ht="96" customHeight="1" thickTop="1" thickBot="1">
       <c r="A30" s="10"/>
       <c r="B30" s="11" t="s">
-        <v>99</v>
+        <v>10</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>19</v>
+        <v>95</v>
       </c>
       <c r="D30" s="11"/>
       <c r="E30" s="12"/>
     </row>
-    <row r="31" spans="1:6" ht="96" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A31" s="10"/>
+    <row r="31" spans="1:6" ht="68" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A31" s="10" t="s">
+        <v>76</v>
+      </c>
       <c r="B31" s="11" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D31" s="11"/>
-      <c r="E31" s="12"/>
-    </row>
-    <row r="32" spans="1:6" ht="68" customHeight="1" thickTop="1" thickBot="1">
+        <v>113</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="96" customHeight="1" thickTop="1" thickBot="1">
       <c r="A32" s="10" t="s">
-        <v>70</v>
+        <v>25</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="E32" s="12" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="60" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A33" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="B33" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C33" s="11" t="s">
+      <c r="D32" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D33" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="F33" s="16"/>
-    </row>
-    <row r="34" spans="1:6" ht="99" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A34" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="B34" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C34" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D34" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="E34" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="F34" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-    </row>
-    <row r="36" spans="1:6" ht="25" customHeight="1">
+      <c r="E32" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F32" s="16"/>
+    </row>
+    <row r="33" spans="1:5" ht="14" thickTop="1">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="1:5" ht="25" customHeight="1">
+      <c r="A34" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+    </row>
+    <row r="35" spans="1:5" ht="21" customHeight="1">
+      <c r="A35" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+    </row>
+    <row r="36" spans="1:5" ht="27" customHeight="1">
       <c r="A36" s="18" t="s">
-        <v>42</v>
+        <v>86</v>
       </c>
       <c r="B36" s="18"/>
       <c r="C36" s="18"/>
       <c r="D36" s="18"/>
       <c r="E36" s="18"/>
     </row>
-    <row r="37" spans="1:6" ht="21" customHeight="1">
-      <c r="A37" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-    </row>
-    <row r="38" spans="1:6" ht="27" customHeight="1">
-      <c r="A38" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-    </row>
-    <row r="40" spans="1:6">
+    <row r="37" spans="1:5">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:5">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:5">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:5">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:5">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:5">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:5">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
     </row>
-    <row r="47" spans="1:6">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="A48" s="3"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+    </row>
+    <row r="48" spans="1:5" ht="16"/>
+    <row r="49" ht="16"/>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="3">
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="A35:E35"/>
     <mergeCell ref="A36:E36"/>
-    <mergeCell ref="A37:E37"/>
-    <mergeCell ref="A38:E38"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75196850393700787" right="0.75196850393700787" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1938,19 +1904,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17" thickBot="1">
       <c r="A1" s="4" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" thickTop="1" thickBot="1">
@@ -1962,65 +1928,64 @@
     </row>
     <row r="3" spans="1:5" ht="90" customHeight="1" thickTop="1" thickBot="1">
       <c r="A3" s="10" t="s">
-        <v>102</v>
+        <v>13</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="12"/>
     </row>
     <row r="4" spans="1:5" ht="79" customHeight="1" thickTop="1" thickBot="1">
       <c r="A4" s="10" t="s">
-        <v>105</v>
+        <v>16</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>100</v>
+        <v>11</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="E4" s="12"/>
     </row>
     <row r="5" spans="1:5" ht="85" customHeight="1" thickTop="1" thickBot="1">
       <c r="A5" s="10" t="s">
-        <v>75</v>
+        <v>33</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>76</v>
+        <v>34</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="12"/>
     </row>
     <row r="6" spans="1:5" ht="106" customHeight="1" thickTop="1" thickBot="1">
       <c r="A6" s="10" t="s">
-        <v>104</v>
+        <v>15</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>38</v>
+        <v>84</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="14" thickTop="1"/>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75196850393700787" right="0.75196850393700787" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -2036,7 +2001,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
@@ -2053,19 +2018,19 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17" thickBot="1">
       <c r="A1" s="4" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" thickTop="1" thickBot="1">
@@ -2077,310 +2042,310 @@
     </row>
     <row r="3" spans="1:7" ht="177" customHeight="1" thickTop="1" thickBot="1">
       <c r="A3" s="10" t="s">
-        <v>45</v>
+        <v>91</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>41</v>
+        <v>87</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="12"/>
     </row>
     <row r="4" spans="1:7" ht="72" customHeight="1" thickTop="1" thickBot="1">
       <c r="A4" s="10" t="s">
-        <v>104</v>
+        <v>15</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A5" s="10" t="s">
-        <v>102</v>
+        <v>13</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>7</v>
+        <v>116</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="12"/>
     </row>
     <row r="6" spans="1:7" ht="121" customHeight="1" thickTop="1" thickBot="1">
       <c r="A6" s="10" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>103</v>
+        <v>14</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>35</v>
+        <v>81</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>119</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="76" customHeight="1" thickTop="1" thickBot="1">
       <c r="A7" s="10" t="s">
-        <v>78</v>
+        <v>36</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>32</v>
+        <v>108</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="12"/>
       <c r="G7" t="s">
-        <v>43</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="150" customHeight="1" thickTop="1" thickBot="1">
       <c r="A8" s="10" t="s">
-        <v>125</v>
+        <v>4</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>122</v>
+        <v>1</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>77</v>
+        <v>35</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="96" customHeight="1" thickTop="1" thickBot="1">
       <c r="A9" s="10"/>
       <c r="B9" s="11" t="s">
-        <v>99</v>
+        <v>10</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>120</v>
+        <v>30</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="12"/>
     </row>
     <row r="10" spans="1:7" ht="142" customHeight="1" thickTop="1" thickBot="1">
       <c r="A10" s="10" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>34</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="66" customHeight="1" thickTop="1" thickBot="1">
       <c r="A11" s="10" t="s">
-        <v>123</v>
+        <v>2</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>44</v>
+        <v>90</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>124</v>
+        <v>3</v>
       </c>
       <c r="F11" s="16"/>
     </row>
     <row r="12" spans="1:7" ht="128" customHeight="1" thickTop="1" thickBot="1">
       <c r="A12" s="10" t="s">
-        <v>101</v>
+        <v>12</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>33</v>
+        <v>79</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="12"/>
     </row>
     <row r="13" spans="1:7" ht="85" customHeight="1" thickTop="1" thickBot="1">
       <c r="A13" s="10" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>84</v>
+        <v>42</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>86</v>
+        <v>44</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>15</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="96" customHeight="1" thickTop="1" thickBot="1">
       <c r="A14" s="10" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>27</v>
+        <v>103</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>28</v>
+        <v>104</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="96" customHeight="1" thickTop="1" thickBot="1">
       <c r="A15" s="10"/>
       <c r="B15" s="11" t="s">
-        <v>99</v>
+        <v>10</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>107</v>
+        <v>18</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="12"/>
     </row>
     <row r="16" spans="1:7" ht="169" customHeight="1" thickTop="1" thickBot="1">
       <c r="A16" s="10" t="s">
-        <v>85</v>
+        <v>43</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>12</v>
+        <v>121</v>
       </c>
       <c r="D16" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="12" t="s">
         <v>82</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>36</v>
       </c>
       <c r="F16" s="16"/>
     </row>
     <row r="17" spans="1:6" ht="55" customHeight="1" thickTop="1" thickBot="1">
       <c r="A17" s="10"/>
       <c r="B17" s="11" t="s">
-        <v>99</v>
+        <v>10</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>108</v>
+        <v>19</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="12"/>
     </row>
     <row r="18" spans="1:6" ht="72" customHeight="1" thickTop="1" thickBot="1">
       <c r="A18" s="10" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>2</v>
+        <v>111</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>14</v>
+        <v>123</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>13</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="55" customHeight="1" thickTop="1" thickBot="1">
       <c r="A19" s="10"/>
       <c r="B19" s="11" t="s">
-        <v>99</v>
+        <v>10</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>109</v>
+        <v>20</v>
       </c>
       <c r="D19" s="11"/>
       <c r="E19" s="12"/>
     </row>
     <row r="20" spans="1:6" ht="95" customHeight="1" thickTop="1" thickBot="1">
       <c r="A20" s="10" t="s">
-        <v>98</v>
+        <v>9</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>29</v>
+        <v>105</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>30</v>
+        <v>106</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="96" customHeight="1" thickTop="1" thickBot="1">
       <c r="A21" s="10"/>
       <c r="B21" s="11" t="s">
-        <v>99</v>
+        <v>10</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>110</v>
+        <v>21</v>
       </c>
       <c r="D21" s="11"/>
       <c r="E21" s="12"/>
     </row>
     <row r="22" spans="1:6" ht="177" customHeight="1" thickTop="1" thickBot="1">
       <c r="A22" s="10" t="s">
-        <v>96</v>
+        <v>7</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>74</v>
+        <v>32</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>73</v>
+        <v>31</v>
       </c>
       <c r="F22" s="16"/>
     </row>
@@ -2394,32 +2359,32 @@
     </row>
     <row r="24" spans="1:6" ht="107" customHeight="1" thickTop="1" thickBot="1">
       <c r="A24" s="10" t="s">
-        <v>79</v>
+        <v>37</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="12"/>
     </row>
     <row r="25" spans="1:6" ht="139" customHeight="1" thickTop="1" thickBot="1">
       <c r="A25" s="10" t="s">
-        <v>80</v>
+        <v>38</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>8</v>
+        <v>117</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>9</v>
+        <v>118</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>10</v>
+        <v>119</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="24" customHeight="1" thickTop="1" thickBot="1">
@@ -2431,13 +2396,13 @@
     </row>
     <row r="27" spans="1:6" ht="67" customHeight="1" thickTop="1" thickBot="1">
       <c r="A27" s="10" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>21</v>
+        <v>97</v>
       </c>
       <c r="D27" s="11"/>
       <c r="E27" s="12"/>
@@ -2445,10 +2410,10 @@
     <row r="28" spans="1:6" ht="70" customHeight="1" thickTop="1" thickBot="1">
       <c r="A28" s="10"/>
       <c r="B28" s="11" t="s">
-        <v>99</v>
+        <v>10</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>117</v>
+        <v>27</v>
       </c>
       <c r="D28" s="11"/>
       <c r="E28" s="12"/>
@@ -2456,67 +2421,67 @@
     <row r="29" spans="1:6" ht="66" customHeight="1" thickTop="1" thickBot="1">
       <c r="A29" s="10"/>
       <c r="B29" s="11" t="s">
-        <v>99</v>
+        <v>10</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>22</v>
+        <v>98</v>
       </c>
       <c r="D29" s="11"/>
       <c r="E29" s="12"/>
     </row>
     <row r="30" spans="1:6" ht="71" customHeight="1" thickTop="1" thickBot="1">
       <c r="A30" s="10" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>0</v>
+        <v>109</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>92</v>
+        <v>50</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="58" customHeight="1" thickTop="1" thickBot="1">
       <c r="A31" s="10" t="s">
-        <v>114</v>
+        <v>25</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>1</v>
+        <v>110</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>93</v>
+        <v>51</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="F31" s="16"/>
     </row>
     <row r="32" spans="1:6" ht="99" customHeight="1" thickTop="1" thickBot="1">
       <c r="A32" s="13" t="s">
-        <v>116</v>
+        <v>26</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>46</v>
+        <v>92</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>47</v>
+        <v>93</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>94</v>
+        <v>52</v>
       </c>
       <c r="F32" t="s">
-        <v>95</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -2528,7 +2493,7 @@
     </row>
     <row r="34" spans="1:5" ht="25" customHeight="1">
       <c r="A34" s="18" t="s">
-        <v>42</v>
+        <v>88</v>
       </c>
       <c r="B34" s="18"/>
       <c r="C34" s="18"/>
@@ -2537,7 +2502,7 @@
     </row>
     <row r="35" spans="1:5" ht="21" customHeight="1">
       <c r="A35" s="18" t="s">
-        <v>39</v>
+        <v>85</v>
       </c>
       <c r="B35" s="18"/>
       <c r="C35" s="18"/>
@@ -2546,7 +2511,7 @@
     </row>
     <row r="36" spans="1:5" ht="27" customHeight="1">
       <c r="A36" s="18" t="s">
-        <v>40</v>
+        <v>86</v>
       </c>
       <c r="B36" s="18"/>
       <c r="C36" s="18"/>
@@ -2630,10 +2595,7 @@
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
     </row>
-    <row r="48" spans="1:5" ht="16"/>
-    <row r="49" ht="16"/>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="3">
     <mergeCell ref="A34:E34"/>
     <mergeCell ref="A35:E35"/>
@@ -2641,7 +2603,6 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75196850393700787" right="0.75196850393700787" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Signal error corrected for VRP example and generator updated. Error (SIG_ABRT) remains in the other two examples. Error stopped incurring after generating correct retrieve calls in a certain occasion.
</commit_message>
<xml_diff>
--- a/EXAMPLES/Examples.xlsx
+++ b/EXAMPLES/Examples.xlsx
@@ -21,7 +21,605 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="138">
+  <si>
+    <t>CREATE TABLE CompanyDB.myVehicles WITH BASE=my_vehicles AS SELECT * FROM map&lt;string,Vehicle&gt;;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE CompanyDB.CPhoneNumber AS SELECT * FROM vector&lt;long int&gt;;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE CompanyDB.EPhoneNumber AS SELECT * FROM vector&lt;long int&gt;;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE TimeDB.Time AS SELECT * FROM tm;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE TimeDB.theTime WITH BASE=theTime AS SELECT * FROM tm*;------------------------------------------------------------------------------- CREATE VIEW TimeDB.TimeView AS SELECT * FROM theTime, Time WHERE Time.base=theTime.time_ptr;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE ELEMENT TABLE Vehicle (plate TEXT FROM plate, brand TEXT FROM get_brand(), model INT FROM model);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE CompanyDB.Fleet AS SELECT * FROM vector&lt;Vehicle&gt;;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE CompanyDB.Location AS SELECT * FROM Address;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE CompanyDB.AddressId AS SELECT * FROM vector&lt;Address*&gt;;----------------------------------------------------- CREATE VIEW CompanyDB.Directory AS SELECT * FROM AddressId, Location WHERE Location.base=AddressId.address_ptr;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE CompanyDB.Home WITH BASE=home AS SELECT * FROM Address;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE CompanyDB.Personnel AS SELECT * FROM vector&lt;Employee&gt;;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE CompanyDB.Evehicle AS SELECT * FROM Vehicle;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE CompanyDB.EmployeeVehicleID AS SELECT * FROM set&lt;Vehicle*&gt;;------------------------------------------------ CREATE VIEW CompanyDB.EmployeeVehicleView AS SELECT * FROM EmployeeVehicleID, EVehicle WHERE EVehicle.base=EmployeeVehicleID.e_vehicle_ptr;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * FROM myVehicles;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE myVehicles (tag_name TEXT, plate TEXT, brand TEXT, model INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * FROM the company, Personnel WHERE Personnel.base = theCompany.c_personnel AND theCompany.name = 'Siemens';</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE ELEMENT TABLE ChessPiece ( name STRING FROM get_name(), color STRING FROM get_color);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE ChessDB.ChessRow AS SELECT * FROM vector&lt;ChessPiece&gt;;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE ChessDB.ChessBoard WITH BASE=chessBoard AS SELECT * FROM vector&lt;vector&lt;ChessPiece&gt; &gt;*;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector&lt;vector&lt;ChessPiece&gt; &gt;* board;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE ELEMENT TABLE ChessBoard (row_id INT FROM self);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE ChessBoard (row_id INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * FROM ChessBoard, ChessRow WHERE ChessRow.base=ChessBoard.row_id AND ChessRow.color="white" and name="bishop";</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE CompanyDB.theCompany WITH BASE=theCompany AS SELECT * FROM Company;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Look for an element table with the same name as the VT irrespective of the type ("AS SELECT * FROM &lt;type&gt;"). If there is no element table (that is no element table name matches (in)type or VT name): search for CREATE ELEMENT TABLE &lt;VTN&gt;.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE ELEMENT TABLE Address (street TEXT FROM get_street(), number TEXT FROM number, postcode TEXT FROM get_postcode());</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE ChessBoard WITH BASE=board AS SELECT * FROM vector&lt;vector&lt;ChessPiece&gt; &gt;;-------</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE ChessRow AS SELECT * FROM vector&lt;ChessPiece&gt;;---------</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CREATE TABLE myVehicles WITH BASE=my_vehicles AS SELECT * FROM map&lt;string,Vehicle&gt;;----------- </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE ELEMENT TABLE Vehicle (plate TEXT FROM plate, brand TEXT FROM get_brand(), model INT FROM model);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE theTime WITH BASE=theTime AS SELECT * FROM tm*;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE theTime (year INT, month INT, day INT, hours INT, minutes INT, seconds INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * FROM theTime;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE AddressId AS SELECT * FROM vector&lt;Address*&gt;;----------------------------------------------------- CREATE VIEW Directory AS SELECT * FROM AddressId, Location WHERE Location.base=AddressId.address_ptr;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE EmployeeVehicleID AS SELECT * FROM set&lt;Vehicle*&gt;;------------------------------------------------ CREATE VIEW EmployeeVehicleView AS SELECT * FROM EmployeeVehicleID, EVehicle WHERE EVehicle.base=EmployeeVehicleID.e_vehicle_ptr;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>A. Object, pointer mismatch for nested stl structs? As defined by user in C++.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE Home (street TEXT, number TEXT, postcode TEXT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>class Company { vector&lt;Vehicle&gt; c_fleet; name string; vector&lt;Address*&gt; c_directory; vat string; vector&lt;Employee&gt; c_personnel; vector&lt;long int&gt;c_phones; }</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE ChessPiece AS SELECT * FROM ChessPiece;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE ChessPiece (base INT, name STRING, color INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE ELEMENT TABLE Employee (name TEXT FROM name, surname TEXT FROM surname, age INT FROM age, e_phones INT FROM get_phones(), e_vehicles FROM get_vehicles());</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE ELEMENT TABLE tm (year INT FROM tm_year, month INT FROM tm_month, day INT FROM tm_mday, hours INT FROM tm_hour, minutes INT FROM tm_min, seconds INT FROM tm_sec);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE ELEMENT TABLE ChessPiece ( name string FROM get_name(), color INT FROM color);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CREATE ELEMENT TABLE ChessBoard (chess_row INT FROM </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>TABLE ChessRow WITH BASE=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>self);</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE ELEMENT TABLE Address (street TEXT FROM get_street(), number TEXT FROM number, postcode TEXT FROM get_postcode());</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mould for pointers to Vehicle element</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE Evehicle AS SELECT * FROM Vehicle;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Record - Table</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE EVehicle (base INT, plate TEXT, brand TEXT, model INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE CPhoneNumber AS SELECT * FROM vector&lt;long int&gt;;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE CPhoneNumber (base INT, phone_number INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>do we support this?work with both built-in base and supplied? The built-in definition has to come first but still. By mixing embedded with stand-alone you disuse the approach used in bestindex to carry out joins in a manner that agrees with our rationale. In conclusion a VT instance is like a constant. It keeps its definition and reflects the same C/C++ entity throughout its lifetime. If it is defined stand-alone, or embedded, it stays that way.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CREATE ELEMENT TABLE Employee (name TEXT FROM name, surname TEXT FROM surname, age INT FROM age, e_phones INT FROM </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>TABLE E_Phone_number WITH BASE=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t xml:space="preserve">get_phones(), e_vehicles FROM </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>TABLE EmployeeVehicleID WITH BASE=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>get_vehicles());</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * FROM theCompany, AddressID, Location WHERE Location.base = AddressId.address_ptr AND AddressId.base = theCompany.c_directory AND theCompany.name = 'Proton Bank';</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT Fleet.plate, Fleet.brand, Fleet.model FROM theCompany,Fleet WHERE Fleet.base = theCompany.c_fleet AND theCompany.name = 'Proton Bank';</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * FROM theCompany, Personnel, EVehicle, EmployeeVehicleID WHERE EVehicle.base=EmployeeVehicleId.e_vehicle_ptr AND EmployeeVehicleID.base = Personnel.e_vehicles AND Personnel.base = theCompany.c_personnel AND theCompany.name = 'Alter' AND Personnel.surname='Giannikos';</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * FROM theTime, Time WHERE time.base = theTime.time_ptr;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE theCompany (c_fleet INT, name TEXT, vat TEXT...);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>B. Namespace for global variables.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C. Use extern global variables all the way or any_dstr?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CREATE ELEMENT TABLE Company (c_fleet INT FROM </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>TABLE Fleet WITH BASE=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t xml:space="preserve">get_fleet(), name TEXT FROM name, c_directory INT FROM </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>TABLE AddressID WITH BASE=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t xml:space="preserve">get_directory(), vat TEXT FROM vat, c_personnel INT FROM </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>TABLE Personnel WITH BASE=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t xml:space="preserve">get_personnel(), c_phones INT FROM </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>TABLE C_Phone_number WITH BASE=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>get_phones());</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE Time (base INT, year INT, month INT, day INT, hours INT, minutes INT, seconds INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE theTime (time_ptr INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE ChessBoard (chess_row INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE ChessRow (base INT, chess_piece INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * FROM ChessBoard, ChessRow, ChessPiece WHERE ChessRow.base=ChessBoard.chess_row AND ChessPiece.base=ChessRow.chess_piece</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SQL CREATE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SQL SELECT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TABLE TYPE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Collection</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Record - Table</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE Home WITH BASE=home AS SELECT * FROM Address;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Record</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE AddressID (base INT, address_ptr INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CREATE ELEMENT TABLE Company (c_fleet INT FROM </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t xml:space="preserve">get_fleet(), name TEXT FROM name, c_directory INT FROM </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t xml:space="preserve">get_directory(), vat TEXT FROM vat, c_personnel INT FROM </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t xml:space="preserve">get_personnel(), c_phones INT FROM </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>get_phones());</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>map&lt;string,Vehicle&gt; my_vehicles;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE theCompany WITH BASE=theCompany AS SELECT * FROM Company;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C++</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DSL</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE Fleet AS SELECT * FROM vector&lt;Vehicle&gt;;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>in class Company: vector&lt;Vehicle&gt; c_fleet;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>in class Company: vector&lt;Address*&gt; c_directory;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>class ChessPiece { string name; int color;}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE theCompany (c_fleet INT, name TEXT, c_directory INT, vat TEXT, c_personnel INT, c_phones INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT theCompany.name FROM theCompany, Fleet WHERE Fleet.base=theCompany.c_fleet AND Fleet.plate LIKE '%99';</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Record</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE Fleet ( base INT, plate TEXT, brand TEXT, model INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE ELEMENT TABLE Vehicle ( plate TEXT FROM plate, brand TEXT FROM get_brand(), model INT FROM model)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector&lt;vector&lt;ChessPiece&gt; &gt; board;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Collection</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>*!*-----type in stl class------- What happens with associative e.g. map&lt;int, Vehicle&gt;?You can override the CREATE ELEMENT TABLE identified by type (explicit command 'USE' &lt;virtual_table_name&gt; right at the bottom of the CREATE TABLE) with CREATE ELEMENT TABLE identified by &lt;virtual_table_name&gt;. To autofill Vehicle we could define "#Vehicle".</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE ELEMENT TABLE AddressId (address_ptr INT FROM self);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT phone_number FROM the company, Personnel, EPhoneNumber WHERE Personnel.base=theCompany.c_personnel AND EPhoneNumber.base=Personnel.e_phones UNION SELECT phone_number FROM the company, CPhoneNumber WHERE CPhoneNumber.base=theCompany.c_phones;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE EPhoneNumber AS SELECT * FROM vector&lt;long int&gt;;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>class Company { vector&lt;Vehicle&gt; c_fleet; name string; vat string;... }</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CREATE ELEMENT TABLE Company ( c_fleet INT </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>FROM TABLE Fleet WITH BASE=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>get_fleet(), name TEXT FROM name, vat TEXT FROM vat;...)</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE Location (base INT, street TEXT, number TEXT, postcode TEXT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>class Address { string street; string number; string postcode; }</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;ctime.h&gt;                   struct tm { int tm_sec; int tm_min; int tm_hour; int tm_mday; int tm_mon; int tm_year;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">#include &lt;ctime.h&gt;        time_t currnt_t=time();   tm *theTime =localtime(currnt_t);                      </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Record - Table</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE EmployeeVehicleID (base INT, e_vehicle_ptr INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>in class Company: vector&lt;Employee&gt; c_personnel;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE Personnel AS SELECT * FROM vector&lt;Employee&gt;;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>in class Employee: set&lt;Vehicle*&gt; e_vehicles;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE VIRTUAL TABLE Personnel (base INT, name TEXT, surname TEXT, age INT, e_phones INT, e_vehicles INT);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mould for pointers to tm element</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Record - Table</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
   <si>
     <t>CREATE ELEMENT TABLE EmployeeVehicleID (e_vehicle_ptr INT FROM self);</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -44,10 +642,6 @@
   </si>
   <si>
     <t>CREATE VIRTUAL TABLE ChessRow (base INT, name STRING, color INT);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE ELEMENT TABLE ChessRow ( name string FROM get_name(), color INT FROM color);</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -160,548 +754,6 @@
   </si>
   <si>
     <t>CREATE ELEMENT TABLE AddressId (address_ptr INT FROM self;)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>*!*-----type in stl class------- What happens with associative e.g. map&lt;int, Vehicle&gt;?You can override the CREATE ELEMENT TABLE identified by type (explicit command 'USE' &lt;virtual_table_name&gt; right at the bottom of the CREATE TABLE) with CREATE ELEMENT TABLE identified by &lt;virtual_table_name&gt;. To autofill Vehicle we could define "#Vehicle".</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE ELEMENT TABLE AddressId (address_ptr INT FROM self);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT phone_number FROM the company, Personnel, EPhoneNumber WHERE Personnel.base=theCompany.c_personnel AND EPhoneNumber.base=Personnel.e_phones UNION SELECT phone_number FROM the company, CPhoneNumber WHERE CPhoneNumber.base=theCompany.c_phones;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE EPhoneNumber AS SELECT * FROM vector&lt;long int&gt;;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>class Company { vector&lt;Vehicle&gt; c_fleet; name string; vat string;... }</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">CREATE ELEMENT TABLE Company ( c_fleet INT </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>FROM TABLE Fleet WITH BASE=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>get_fleet(), name TEXT FROM name, vat TEXT FROM vat;...)</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE Location (base INT, street TEXT, number TEXT, postcode TEXT);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>class Address { string street; string number; string postcode; }</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;ctime.h&gt;                   struct tm { int tm_sec; int tm_min; int tm_hour; int tm_mday; int tm_mon; int tm_year;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">#include &lt;ctime.h&gt;        time_t currnt_t=time();   tm *theTime =localtime(currnt_t);                      </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Record - Table</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE EmployeeVehicleID (base INT, e_vehicle_ptr INT);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>in class Company: vector&lt;Employee&gt; c_personnel;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE Personnel AS SELECT * FROM vector&lt;Employee&gt;;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>in class Employee: set&lt;Vehicle*&gt; e_vehicles;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE Personnel (base INT, name TEXT, surname TEXT, age INT, e_phones INT, e_vehicles INT);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>mould for pointers to tm element</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Record - Table</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE Time AS SELECT * FROM tm;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE Time (base INT, year INT, month INT, day INT, hours INT, minutes INT, seconds INT);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE theTime (time_ptr INT);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE ChessBoard (chess_row INT);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE ChessRow (base INT, chess_piece INT);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT * FROM ChessBoard, ChessRow, ChessPiece WHERE ChessRow.base=ChessBoard.chess_row AND ChessPiece.base=ChessRow.chess_piece</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SQL CREATE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SQL SELECT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>TABLE TYPE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Collection</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Record - Table</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE Home WITH BASE=home AS SELECT * FROM Address;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Record</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE AddressID (base INT, address_ptr INT);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">CREATE ELEMENT TABLE Company (c_fleet INT FROM </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t xml:space="preserve">get_fleet(), name TEXT FROM name, c_directory INT FROM </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t xml:space="preserve">get_directory(), vat TEXT FROM vat, c_personnel INT FROM </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t xml:space="preserve">get_personnel(), c_phones INT FROM </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>get_phones());</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>map&lt;string,Vehicle&gt; my_vehicles;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE theCompany WITH BASE=theCompany AS SELECT * FROM Company;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>C++</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>DSL</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE Fleet AS SELECT * FROM vector&lt;Vehicle&gt;;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>in class Company: vector&lt;Vehicle&gt; c_fleet;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>in class Company: vector&lt;Address*&gt; c_directory;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>class ChessPiece { string name; int color;}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE theCompany (c_fleet INT, name TEXT, c_directory INT, vat TEXT, c_personnel INT, c_phones INT);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT theCompany.name FROM theCompany, Fleet WHERE Fleet.base=theCompany.c_fleet AND Fleet.plate LIKE '%99';</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Record</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE Fleet ( base INT, plate TEXT, brand TEXT, model INT);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE ELEMENT TABLE Vehicle ( plate TEXT FROM plate, brand TEXT FROM get_brand(), model INT FROM model)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>vector&lt;vector&lt;ChessPiece&gt; &gt; board;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Collection</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>do we support this?work with both built-in base and supplied? The built-in definition has to come first but still. By mixing embedded with stand-alone you disuse the approach used in bestindex to carry out joins in a manner that agrees with our rationale. In conclusion a VT instance is like a constant. It keeps its definition and reflects the same C/C++ entity throughout its lifetime. If it is defined stand-alone, or embedded, it stays that way.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">CREATE ELEMENT TABLE Employee (name TEXT FROM name, surname TEXT FROM surname, age INT FROM age, e_phones INT FROM </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>TABLE E_Phone_number WITH BASE=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t xml:space="preserve">get_phones(), e_vehicles FROM </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>TABLE EmployeeVehicleID WITH BASE=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>get_vehicles());</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT * FROM theCompany, AddressID, Location WHERE Location.base = AddressId.address_ptr AND AddressId.base = theCompany.c_directory AND theCompany.name = 'Proton Bank';</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT Fleet.plate, Fleet.brand, Fleet.model FROM theCompany,Fleet WHERE Fleet.base = theCompany.c_fleet AND theCompany.name = 'Proton Bank';</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT * FROM theCompany, Personnel, EVehicle, EmployeeVehicleID WHERE EVehicle.base=EmployeeVehicleId.e_vehicle_ptr AND EmployeeVehicleID.base = Personnel.e_vehicles AND Personnel.base = theCompany.c_personnel AND theCompany.name = 'Alter' AND Personnel.surname='Giannikos';</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT * FROM theTime, Time WHERE time.base = theTime.time_ptr;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE theCompany (c_fleet INT, name TEXT, vat TEXT...);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>B. Namespace for global variables.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>C. Use extern global variables all the way or any_dstr?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">CREATE ELEMENT TABLE Company (c_fleet INT FROM </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>TABLE Fleet WITH BASE=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t xml:space="preserve">get_fleet(), name TEXT FROM name, c_directory INT FROM </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>TABLE AddressID WITH BASE=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t xml:space="preserve">get_directory(), vat TEXT FROM vat, c_personnel INT FROM </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>TABLE Personnel WITH BASE=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t xml:space="preserve">get_personnel(), c_phones INT FROM </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>TABLE C_Phone_number WITH BASE=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>get_phones());</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>A. Object, pointer mismatch for nested stl structs? As defined by user in C++.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE Home (street TEXT, number TEXT, postcode TEXT);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>class Company { vector&lt;Vehicle&gt; c_fleet; name string; vector&lt;Address*&gt; c_directory; vat string; vector&lt;Employee&gt; c_personnel; vector&lt;long int&gt;c_phones; }</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE ChessPiece AS SELECT * FROM ChessPiece;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE ChessPiece (base INT, name STRING, color INT);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE ELEMENT TABLE Employee (name TEXT FROM name, surname TEXT FROM surname, age INT FROM age, e_phones INT FROM get_phones(), e_vehicles FROM get_vehicles());</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE ELEMENT TABLE ChessBoard (chess_row INT FROM self);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE ELEMENT TABLE tm (year INT FROM tm_year, month INT FROM tm_month, day INT FROM tm_mday, hours INT FROM tm_hour, minutes INT FROM tm_min, seconds INT FROM tm_sec);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE ELEMENT TABLE ChessPiece ( name string FROM get_name(), color INT FROM color);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">CREATE ELEMENT TABLE ChessBoard (chess_row INT FROM </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>TABLE ChessRow WITH BASE=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>self);</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE ELEMENT TABLE Vehicle (plate TEXT FROM plate, brand TEXT FROM get_brand(), model INT FROM model);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE ELEMENT TABLE Address (street TEXT FROM get_street(), number TEXT FROM number, postcode TEXT FROM get_postcode());</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>mould for pointers to Vehicle element</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE Evehicle AS SELECT * FROM Vehicle;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Record - Table</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE EVehicle (base INT, plate TEXT, brand TEXT, model INT);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE CPhoneNumber AS SELECT * FROM vector&lt;long int&gt;;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE CPhoneNumber (base INT, phone_number INT);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Look for an element table with the same name as the VT irrespective of the type ("AS SELECT * FROM &lt;type&gt;"). If there is no element table (that is no element table name matches (in)type or VT name): search for CREATE ELEMENT TABLE &lt;VTN&gt;.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE ELEMENT TABLE Address (street TEXT FROM get_street(), number TEXT FROM number, postcode TEXT FROM get_postcode());</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE ChessBoard WITH BASE=board AS SELECT * FROM vector&lt;vector&lt;ChessPiece&gt; &gt;;-------</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE ChessRow AS SELECT * FROM vector&lt;ChessPiece&gt;;---------</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">CREATE TABLE myVehicles WITH BASE=my_vehicles AS SELECT * FROM map&lt;string,Vehicle&gt;;----------- </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE theTime WITH BASE=theTime AS SELECT * FROM tm*;------------------------------------------------------------------------------- CREATE VIEW TimeView AS SELECT * FROM theTime, Time WHERE Time.base=theTime.time_ptr;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE ChessBoard WITH BASE=board AS SELECT * FROM vector&lt;vector&lt;ChessPiece&gt; &gt;;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE ChessRow AS SELECT * FROM vector&lt;ChessPiece&gt;;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE myVehicles WITH BASE=my_vehicles AS SELECT * FROM map&lt;string,Vehicle&gt;;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE ELEMENT TABLE Vehicle (plate TEXT FROM plate, brand TEXT FROM get_brand(), model INT FROM model);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE theTime WITH BASE=theTime AS SELECT * FROM tm*;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE theTime (year INT, month INT, day INT, hours INT, minutes INT, seconds INT);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT * FROM theTime;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE AddressId AS SELECT * FROM vector&lt;Address*&gt;;----------------------------------------------------- CREATE VIEW Directory AS SELECT * FROM AddressId, Location WHERE Location.base=AddressId.address_ptr;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE EmployeeVehicleID AS SELECT * FROM set&lt;Vehicle*&gt;;------------------------------------------------ CREATE VIEW EmployeeVehicleView AS SELECT * FROM EmployeeVehicleID, EVehicle WHERE EVehicle.base=EmployeeVehicleID.e_vehicle_ptr;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT * FROM myVehicles;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE VIRTUAL TABLE myVehicles (tag_name TEXT, plate TEXT, brand TEXT, model INT);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT * FROM the company, Personnel WHERE Personnel.base = theCompany.c_personnel AND theCompany.name = 'Siemens';</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1272,10 +1324,10 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:XFD30"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1289,19 +1341,19 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17" thickBot="1">
       <c r="A1" s="4" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" thickTop="1" thickBot="1">
@@ -1313,310 +1365,310 @@
     </row>
     <row r="3" spans="1:7" ht="121" customHeight="1" thickTop="1" thickBot="1">
       <c r="A3" s="10" t="s">
-        <v>91</v>
+        <v>38</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="12"/>
     </row>
     <row r="4" spans="1:7" ht="71" customHeight="1" thickTop="1" thickBot="1">
       <c r="A4" s="10" t="s">
-        <v>15</v>
+        <v>124</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>64</v>
+        <v>23</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="71" customHeight="1" thickTop="1" thickBot="1">
       <c r="A5" s="10" t="s">
-        <v>13</v>
+        <v>122</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>99</v>
+        <v>5</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="12"/>
     </row>
     <row r="6" spans="1:7" ht="123" customHeight="1" thickTop="1" thickBot="1">
       <c r="A6" s="10" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>67</v>
+        <v>6</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>14</v>
+        <v>123</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>29</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="86" customHeight="1" thickTop="1" thickBot="1">
       <c r="A7" s="10" t="s">
-        <v>36</v>
+        <v>99</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>100</v>
+        <v>45</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="12"/>
       <c r="G7" t="s">
-        <v>89</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="132" thickTop="1" thickBot="1">
       <c r="A8" s="10" t="s">
-        <v>4</v>
+        <v>114</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>35</v>
+        <v>98</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>8</v>
+        <v>117</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>78</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="49" customHeight="1" thickTop="1" thickBot="1">
       <c r="A9" s="10"/>
       <c r="B9" s="11" t="s">
-        <v>10</v>
+        <v>119</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>28</v>
+        <v>137</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="12"/>
     </row>
     <row r="10" spans="1:7" ht="136" customHeight="1" thickTop="1" thickBot="1">
       <c r="A10" s="10" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>120</v>
+        <v>8</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="58" customHeight="1" thickTop="1" thickBot="1">
       <c r="A11" s="10" t="s">
-        <v>2</v>
+        <v>112</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>90</v>
+        <v>37</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>3</v>
+        <v>113</v>
       </c>
       <c r="F11" s="16"/>
     </row>
     <row r="12" spans="1:7" ht="102" customHeight="1" thickTop="1" thickBot="1">
       <c r="A12" s="10" t="s">
-        <v>12</v>
+        <v>121</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>94</v>
+        <v>41</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="12"/>
     </row>
     <row r="13" spans="1:7" ht="85" customHeight="1" thickTop="1" thickBot="1">
       <c r="A13" s="10" t="s">
-        <v>41</v>
+        <v>104</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>44</v>
+        <v>107</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>124</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="58" customHeight="1" thickTop="1" thickBot="1">
       <c r="A14" s="10" t="s">
-        <v>101</v>
+        <v>46</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>103</v>
+        <v>48</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>102</v>
+        <v>11</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>104</v>
+        <v>49</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>8</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="60" customHeight="1" thickTop="1" thickBot="1">
       <c r="A15" s="10"/>
       <c r="B15" s="11" t="s">
-        <v>10</v>
+        <v>119</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="12"/>
     </row>
     <row r="16" spans="1:7" ht="165" customHeight="1" thickTop="1" thickBot="1">
       <c r="A16" s="10" t="s">
-        <v>43</v>
+        <v>106</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>121</v>
+        <v>12</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>40</v>
+        <v>103</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>82</v>
+        <v>56</v>
       </c>
       <c r="F16" s="16"/>
     </row>
     <row r="17" spans="1:6" ht="55" customHeight="1" thickTop="1" thickBot="1">
       <c r="A17" s="10"/>
       <c r="B17" s="11" t="s">
-        <v>10</v>
+        <v>119</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>17</v>
+        <v>126</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="12"/>
     </row>
     <row r="18" spans="1:6" ht="72" customHeight="1" thickTop="1" thickBot="1">
       <c r="A18" s="10" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>115</v>
+        <v>0</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>123</v>
+        <v>14</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>122</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="55" customHeight="1" thickTop="1" thickBot="1">
       <c r="A19" s="10"/>
       <c r="B19" s="11" t="s">
-        <v>10</v>
+        <v>119</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>23</v>
+        <v>132</v>
       </c>
       <c r="D19" s="11"/>
       <c r="E19" s="12"/>
     </row>
     <row r="20" spans="1:6" ht="95" customHeight="1" thickTop="1" thickBot="1">
       <c r="A20" s="10" t="s">
-        <v>9</v>
+        <v>118</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>106</v>
+        <v>51</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>8</v>
+        <v>117</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>107</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="66" customHeight="1" thickTop="1" thickBot="1">
       <c r="A21" s="10"/>
       <c r="B21" s="11" t="s">
-        <v>10</v>
+        <v>119</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>21</v>
+        <v>130</v>
       </c>
       <c r="D21" s="11"/>
       <c r="E21" s="12"/>
     </row>
     <row r="22" spans="1:6" ht="166" customHeight="1" thickTop="1" thickBot="1">
       <c r="A22" s="10" t="s">
-        <v>7</v>
+        <v>116</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>24</v>
+        <v>133</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>31</v>
+        <v>94</v>
       </c>
       <c r="F22" s="16"/>
     </row>
@@ -1630,60 +1682,60 @@
     </row>
     <row r="24" spans="1:6" ht="107" customHeight="1" thickTop="1" thickBot="1">
       <c r="A24" s="10" t="s">
-        <v>37</v>
+        <v>100</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>96</v>
+        <v>42</v>
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="12"/>
     </row>
     <row r="25" spans="1:6" ht="70" customHeight="1" thickTop="1" thickBot="1">
       <c r="A25" s="10" t="s">
-        <v>45</v>
+        <v>108</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>46</v>
+        <v>109</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>47</v>
+        <v>3</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>8</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="96" customHeight="1" thickTop="1" thickBot="1">
       <c r="A26" s="10"/>
       <c r="B26" s="11" t="s">
-        <v>10</v>
+        <v>119</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>22</v>
+        <v>131</v>
       </c>
       <c r="D26" s="11"/>
       <c r="E26" s="12"/>
     </row>
     <row r="27" spans="1:6" ht="139" customHeight="1" thickTop="1" thickBot="1">
       <c r="A27" s="10" t="s">
-        <v>38</v>
+        <v>101</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>112</v>
+        <v>4</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="24" customHeight="1" thickTop="1" thickBot="1">
@@ -1695,13 +1747,13 @@
     </row>
     <row r="29" spans="1:6" ht="96" customHeight="1" thickTop="1" thickBot="1">
       <c r="A29" s="10" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D29" s="11"/>
       <c r="E29" s="12"/>
@@ -1709,46 +1761,46 @@
     <row r="30" spans="1:6" ht="96" customHeight="1" thickTop="1" thickBot="1">
       <c r="A30" s="10"/>
       <c r="B30" s="11" t="s">
-        <v>10</v>
+        <v>119</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>95</v>
+        <v>20</v>
       </c>
       <c r="D30" s="11"/>
       <c r="E30" s="12"/>
     </row>
     <row r="31" spans="1:6" ht="68" customHeight="1" thickTop="1" thickBot="1">
       <c r="A31" s="10" t="s">
-        <v>76</v>
+        <v>19</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>113</v>
+        <v>18</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>8</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="96" customHeight="1" thickTop="1" thickBot="1">
       <c r="A32" s="10" t="s">
-        <v>25</v>
+        <v>134</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>114</v>
+        <v>17</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>5</v>
+        <v>115</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="F32" s="16"/>
     </row>
@@ -1761,7 +1813,7 @@
     </row>
     <row r="34" spans="1:5" ht="25" customHeight="1">
       <c r="A34" s="18" t="s">
-        <v>88</v>
+        <v>35</v>
       </c>
       <c r="B34" s="18"/>
       <c r="C34" s="18"/>
@@ -1770,7 +1822,7 @@
     </row>
     <row r="35" spans="1:5" ht="21" customHeight="1">
       <c r="A35" s="18" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="B35" s="18"/>
       <c r="C35" s="18"/>
@@ -1779,7 +1831,7 @@
     </row>
     <row r="36" spans="1:5" ht="27" customHeight="1">
       <c r="A36" s="18" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="B36" s="18"/>
       <c r="C36" s="18"/>
@@ -1863,8 +1915,6 @@
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
     </row>
-    <row r="48" spans="1:5" ht="16"/>
-    <row r="49" ht="16"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A34:E34"/>
@@ -1873,7 +1923,6 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75196850393700787" right="0.75196850393700787" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" scale="39" fitToHeight="2" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1904,19 +1953,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17" thickBot="1">
       <c r="A1" s="4" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" thickTop="1" thickBot="1">
@@ -1928,60 +1977,60 @@
     </row>
     <row r="3" spans="1:5" ht="90" customHeight="1" thickTop="1" thickBot="1">
       <c r="A3" s="10" t="s">
-        <v>13</v>
+        <v>122</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="12"/>
     </row>
     <row r="4" spans="1:5" ht="79" customHeight="1" thickTop="1" thickBot="1">
       <c r="A4" s="10" t="s">
-        <v>16</v>
+        <v>125</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="E4" s="12"/>
     </row>
     <row r="5" spans="1:5" ht="85" customHeight="1" thickTop="1" thickBot="1">
       <c r="A5" s="10" t="s">
-        <v>33</v>
+        <v>96</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>34</v>
+        <v>97</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="12"/>
     </row>
     <row r="6" spans="1:5" ht="106" customHeight="1" thickTop="1" thickBot="1">
       <c r="A6" s="10" t="s">
-        <v>15</v>
+        <v>124</v>
       </c>
       <c r="B6" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>84</v>
-      </c>
       <c r="E6" s="12" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="14" thickTop="1"/>
@@ -2018,19 +2067,19 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17" thickBot="1">
       <c r="A1" s="4" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" thickTop="1" thickBot="1">
@@ -2042,310 +2091,310 @@
     </row>
     <row r="3" spans="1:7" ht="177" customHeight="1" thickTop="1" thickBot="1">
       <c r="A3" s="10" t="s">
-        <v>91</v>
+        <v>38</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>87</v>
+        <v>61</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="12"/>
     </row>
     <row r="4" spans="1:7" ht="72" customHeight="1" thickTop="1" thickBot="1">
       <c r="A4" s="10" t="s">
-        <v>15</v>
+        <v>124</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A5" s="10" t="s">
-        <v>13</v>
+        <v>122</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>116</v>
+        <v>29</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="12"/>
     </row>
     <row r="6" spans="1:7" ht="121" customHeight="1" thickTop="1" thickBot="1">
       <c r="A6" s="10" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>14</v>
+        <v>123</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>29</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="76" customHeight="1" thickTop="1" thickBot="1">
       <c r="A7" s="10" t="s">
-        <v>36</v>
+        <v>99</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>108</v>
+        <v>25</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="12"/>
       <c r="G7" t="s">
-        <v>89</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="150" customHeight="1" thickTop="1" thickBot="1">
       <c r="A8" s="10" t="s">
-        <v>4</v>
+        <v>114</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>35</v>
+        <v>98</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>8</v>
+        <v>117</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>78</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="96" customHeight="1" thickTop="1" thickBot="1">
       <c r="A9" s="10"/>
       <c r="B9" s="11" t="s">
-        <v>10</v>
+        <v>119</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>30</v>
+        <v>93</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="12"/>
     </row>
     <row r="10" spans="1:7" ht="142" customHeight="1" thickTop="1" thickBot="1">
       <c r="A10" s="10" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>120</v>
+        <v>33</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="66" customHeight="1" thickTop="1" thickBot="1">
       <c r="A11" s="10" t="s">
-        <v>2</v>
+        <v>112</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>90</v>
+        <v>37</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>3</v>
+        <v>113</v>
       </c>
       <c r="F11" s="16"/>
     </row>
     <row r="12" spans="1:7" ht="128" customHeight="1" thickTop="1" thickBot="1">
       <c r="A12" s="10" t="s">
-        <v>12</v>
+        <v>121</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="12"/>
     </row>
     <row r="13" spans="1:7" ht="85" customHeight="1" thickTop="1" thickBot="1">
       <c r="A13" s="10" t="s">
-        <v>41</v>
+        <v>104</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>42</v>
+        <v>105</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>44</v>
+        <v>107</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>124</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="96" customHeight="1" thickTop="1" thickBot="1">
       <c r="A14" s="10" t="s">
-        <v>101</v>
+        <v>46</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>103</v>
+        <v>48</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>102</v>
+        <v>47</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>104</v>
+        <v>49</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>8</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="96" customHeight="1" thickTop="1" thickBot="1">
       <c r="A15" s="10"/>
       <c r="B15" s="11" t="s">
-        <v>10</v>
+        <v>119</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>18</v>
+        <v>127</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="12"/>
     </row>
     <row r="16" spans="1:7" ht="169" customHeight="1" thickTop="1" thickBot="1">
       <c r="A16" s="10" t="s">
-        <v>43</v>
+        <v>106</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>121</v>
+        <v>34</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>40</v>
+        <v>103</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>82</v>
+        <v>56</v>
       </c>
       <c r="F16" s="16"/>
     </row>
     <row r="17" spans="1:6" ht="55" customHeight="1" thickTop="1" thickBot="1">
       <c r="A17" s="10"/>
       <c r="B17" s="11" t="s">
-        <v>10</v>
+        <v>119</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>19</v>
+        <v>128</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="12"/>
     </row>
     <row r="18" spans="1:6" ht="72" customHeight="1" thickTop="1" thickBot="1">
       <c r="A18" s="10" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>111</v>
+        <v>28</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>123</v>
+        <v>14</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>122</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="55" customHeight="1" thickTop="1" thickBot="1">
       <c r="A19" s="10"/>
       <c r="B19" s="11" t="s">
-        <v>10</v>
+        <v>119</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>20</v>
+        <v>129</v>
       </c>
       <c r="D19" s="11"/>
       <c r="E19" s="12"/>
     </row>
     <row r="20" spans="1:6" ht="95" customHeight="1" thickTop="1" thickBot="1">
       <c r="A20" s="10" t="s">
-        <v>9</v>
+        <v>118</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>105</v>
+        <v>50</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>106</v>
+        <v>51</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>8</v>
+        <v>117</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>107</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="96" customHeight="1" thickTop="1" thickBot="1">
       <c r="A21" s="10"/>
       <c r="B21" s="11" t="s">
-        <v>10</v>
+        <v>119</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>21</v>
+        <v>130</v>
       </c>
       <c r="D21" s="11"/>
       <c r="E21" s="12"/>
     </row>
     <row r="22" spans="1:6" ht="177" customHeight="1" thickTop="1" thickBot="1">
       <c r="A22" s="10" t="s">
-        <v>7</v>
+        <v>116</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>32</v>
+        <v>95</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>24</v>
+        <v>133</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>31</v>
+        <v>94</v>
       </c>
       <c r="F22" s="16"/>
     </row>
@@ -2359,32 +2408,32 @@
     </row>
     <row r="24" spans="1:6" ht="107" customHeight="1" thickTop="1" thickBot="1">
       <c r="A24" s="10" t="s">
-        <v>37</v>
+        <v>100</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>96</v>
+        <v>42</v>
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="12"/>
     </row>
     <row r="25" spans="1:6" ht="139" customHeight="1" thickTop="1" thickBot="1">
       <c r="A25" s="10" t="s">
-        <v>38</v>
+        <v>101</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>117</v>
+        <v>30</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>118</v>
+        <v>31</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>119</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="24" customHeight="1" thickTop="1" thickBot="1">
@@ -2396,13 +2445,13 @@
     </row>
     <row r="27" spans="1:6" ht="67" customHeight="1" thickTop="1" thickBot="1">
       <c r="A27" s="10" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>97</v>
+        <v>43</v>
       </c>
       <c r="D27" s="11"/>
       <c r="E27" s="12"/>
@@ -2410,10 +2459,10 @@
     <row r="28" spans="1:6" ht="70" customHeight="1" thickTop="1" thickBot="1">
       <c r="A28" s="10"/>
       <c r="B28" s="11" t="s">
-        <v>10</v>
+        <v>119</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>27</v>
+        <v>136</v>
       </c>
       <c r="D28" s="11"/>
       <c r="E28" s="12"/>
@@ -2421,67 +2470,67 @@
     <row r="29" spans="1:6" ht="66" customHeight="1" thickTop="1" thickBot="1">
       <c r="A29" s="10"/>
       <c r="B29" s="11" t="s">
-        <v>10</v>
+        <v>119</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>98</v>
+        <v>44</v>
       </c>
       <c r="D29" s="11"/>
       <c r="E29" s="12"/>
     </row>
     <row r="30" spans="1:6" ht="71" customHeight="1" thickTop="1" thickBot="1">
       <c r="A30" s="10" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>109</v>
+        <v>26</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>8</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="58" customHeight="1" thickTop="1" thickBot="1">
       <c r="A31" s="10" t="s">
-        <v>25</v>
+        <v>134</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>110</v>
+        <v>27</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>8</v>
+        <v>117</v>
       </c>
       <c r="F31" s="16"/>
     </row>
     <row r="32" spans="1:6" ht="99" customHeight="1" thickTop="1" thickBot="1">
       <c r="A32" s="13" t="s">
-        <v>26</v>
+        <v>135</v>
       </c>
       <c r="B32" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="C32" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C32" s="14" t="s">
-        <v>92</v>
-      </c>
       <c r="D32" s="14" t="s">
-        <v>93</v>
+        <v>40</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="F32" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -2493,7 +2542,7 @@
     </row>
     <row r="34" spans="1:5" ht="25" customHeight="1">
       <c r="A34" s="18" t="s">
-        <v>88</v>
+        <v>35</v>
       </c>
       <c r="B34" s="18"/>
       <c r="C34" s="18"/>
@@ -2502,7 +2551,7 @@
     </row>
     <row r="35" spans="1:5" ht="21" customHeight="1">
       <c r="A35" s="18" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="B35" s="18"/>
       <c r="C35" s="18"/>
@@ -2511,7 +2560,7 @@
     </row>
     <row r="36" spans="1:5" ht="27" customHeight="1">
       <c r="A36" s="18" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="B36" s="18"/>
       <c r="C36" s="18"/>

</xml_diff>